<commit_message>
assignment 3 code finished
</commit_message>
<xml_diff>
--- a/assignment_3/assignment_3.xlsx
+++ b/assignment_3/assignment_3.xlsx
@@ -198,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -479,11 +479,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -533,6 +572,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -557,10 +610,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -569,26 +622,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,7 +731,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -709,89 +761,95 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>problem1!$B$16:$B$26</c:f>
+              <c:f>problem1!$B$16:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2</c:v>
+                  <c:v>0.15000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>0.44999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6</c:v>
+                  <c:v>0.54999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.7</c:v>
+                  <c:v>0.64999999999999991</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79999999999999993</c:v>
+                  <c:v>0.74999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.89999999999999991</c:v>
+                  <c:v>0.84999999999999987</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999989</c:v>
+                  <c:v>0.94999999999999984</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>problem1!$C$16:$C$26</c:f>
+              <c:f>problem1!$C$16:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8432310820697546E-20</c:v>
+                  <c:v>2.1568233526564253E-21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2481613803067933E-18</c:v>
+                  <c:v>3.485332782146486E-19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3051148313971531E-16</c:v>
+                  <c:v>5.1755357183033894E-17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3576229495526771E-14</c:v>
+                  <c:v>7.6812044923271107E-15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3887943864771149E-11</c:v>
+                  <c:v>1.1399918528514765E-12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0611536224383651E-9</c:v>
+                  <c:v>1.6918979226131959E-10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0590232050182563E-7</c:v>
+                  <c:v>2.5109991557439448E-8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5399929762484861E-5</c:v>
+                  <c:v>3.7266531720786451E-6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.7379469990854202E-3</c:v>
+                  <c:v>5.5308437014782972E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99999999999999289</c:v>
+                  <c:v>8.2084998623898217E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8EAD-4668-8EBC-D620D2F24882}"/>
@@ -1081,144 +1139,150 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>problem1!$D$16:$D$36</c:f>
+              <c:f>problem1!$D$16:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.05</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1</c:v>
+                  <c:v>7.5000000000000011E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15000000000000002</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2</c:v>
+                  <c:v>0.17499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.25</c:v>
+                  <c:v>0.22499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.3</c:v>
+                  <c:v>0.27499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.35</c:v>
+                  <c:v>0.32499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39999999999999997</c:v>
+                  <c:v>0.37499999999999994</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.44999999999999996</c:v>
+                  <c:v>0.42499999999999993</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.49999999999999994</c:v>
+                  <c:v>0.47499999999999992</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.54999999999999993</c:v>
+                  <c:v>0.52499999999999991</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.6</c:v>
+                  <c:v>0.57499999999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.65</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.70000000000000007</c:v>
+                  <c:v>0.67500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.75000000000000011</c:v>
+                  <c:v>0.72500000000000009</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.80000000000000016</c:v>
+                  <c:v>0.77500000000000013</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.8500000000000002</c:v>
+                  <c:v>0.82500000000000018</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.90000000000000024</c:v>
+                  <c:v>0.87500000000000022</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.95000000000000029</c:v>
+                  <c:v>0.92500000000000027</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.0000000000000002</c:v>
+                  <c:v>0.97500000000000031</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>problem1!$E$16:$E$36</c:f>
+              <c:f>problem1!$E$16:$E$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1568233526564253E-21</c:v>
+                  <c:v>4.8032486005825407E-22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8432310820697546E-20</c:v>
+                  <c:v>8.0083780594918503E-21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.485332782146486E-19</c:v>
+                  <c:v>9.9718840697446029E-20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2481613803067933E-18</c:v>
+                  <c:v>1.2169809979176447E-18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.1755357183033894E-17</c:v>
+                  <c:v>1.4828020480775224E-17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.3051148313971422E-16</c:v>
+                  <c:v>1.8064442677958422E-16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.6812044923271107E-15</c:v>
+                  <c:v>2.2007017951003744E-15</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3576229495526771E-14</c:v>
+                  <c:v>2.6810038484942956E-14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1399918528514765E-12</c:v>
+                  <c:v>3.2661313408586857E-13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3887943864771099E-11</c:v>
+                  <c:v>3.9789625356443517E-12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.6918979226131959E-10</c:v>
+                  <c:v>4.8473687062509513E-11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.0611536224383651E-9</c:v>
+                  <c:v>5.9053039989420903E-10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.5109991557439627E-8</c:v>
+                  <c:v>7.1941330303251907E-9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.0590232050182563E-7</c:v>
+                  <c:v>8.7642482194436174E-8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.7266531720786976E-6</c:v>
+                  <c:v>1.0677040100347901E-6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.5399929762485179E-5</c:v>
+                  <c:v>1.3007297654067714E-5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.5308437014783753E-4</c:v>
+                  <c:v>1.5846132511575239E-4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.7379469990855633E-3</c:v>
+                  <c:v>1.9304541362277371E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.2084998623899966E-2</c:v>
+                  <c:v>2.3517745856009444E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.0000000000000144</c:v>
+                  <c:v>0.2865047968601942</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1513,264 +1577,270 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>problem1!$F$16:$F$56</c:f>
+              <c:f>problem1!$F$16:$F$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>1.2500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.05</c:v>
+                  <c:v>3.7500000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.5000000000000011E-2</c:v>
+                  <c:v>6.25E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1</c:v>
+                  <c:v>8.7499999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.125</c:v>
+                  <c:v>0.11249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.15</c:v>
+                  <c:v>0.13749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17499999999999999</c:v>
+                  <c:v>0.16249999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.19999999999999998</c:v>
+                  <c:v>0.18749999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.22499999999999998</c:v>
+                  <c:v>0.21249999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.24999999999999997</c:v>
+                  <c:v>0.23749999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.27499999999999997</c:v>
+                  <c:v>0.26249999999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.3</c:v>
+                  <c:v>0.28749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.32500000000000001</c:v>
+                  <c:v>0.3125</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.35000000000000003</c:v>
+                  <c:v>0.33750000000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.37500000000000006</c:v>
+                  <c:v>0.36250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.40000000000000008</c:v>
+                  <c:v>0.38750000000000007</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.4250000000000001</c:v>
+                  <c:v>0.41250000000000009</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.45000000000000012</c:v>
+                  <c:v>0.43750000000000011</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.47500000000000014</c:v>
+                  <c:v>0.46250000000000013</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.50000000000000011</c:v>
+                  <c:v>0.48750000000000016</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.52500000000000013</c:v>
+                  <c:v>0.51250000000000018</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.55000000000000016</c:v>
+                  <c:v>0.5375000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.57500000000000018</c:v>
+                  <c:v>0.56250000000000022</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.6000000000000002</c:v>
+                  <c:v>0.58750000000000024</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.62500000000000022</c:v>
+                  <c:v>0.61250000000000027</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.65000000000000024</c:v>
+                  <c:v>0.63750000000000029</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.67500000000000027</c:v>
+                  <c:v>0.66250000000000031</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.70000000000000029</c:v>
+                  <c:v>0.68750000000000033</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.72500000000000031</c:v>
+                  <c:v>0.71250000000000036</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.75000000000000033</c:v>
+                  <c:v>0.73750000000000038</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.77500000000000036</c:v>
+                  <c:v>0.7625000000000004</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.80000000000000038</c:v>
+                  <c:v>0.78750000000000042</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.8250000000000004</c:v>
+                  <c:v>0.81250000000000044</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.85000000000000042</c:v>
+                  <c:v>0.83750000000000047</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.87500000000000044</c:v>
+                  <c:v>0.86250000000000049</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.90000000000000047</c:v>
+                  <c:v>0.88750000000000051</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.92500000000000049</c:v>
+                  <c:v>0.91250000000000053</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.95000000000000051</c:v>
+                  <c:v>0.93750000000000056</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.97500000000000053</c:v>
+                  <c:v>0.96250000000000058</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.0000000000000004</c:v>
+                  <c:v>0.9875000000000006</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0000000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>problem1!$G$16:$G$56</c:f>
+              <c:f>problem1!$G$16:$G$57</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8032486005825407E-22</c:v>
+                  <c:v>1.6746292583926853E-22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1568233526564253E-21</c:v>
+                  <c:v>1.0648279038972999E-21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0083780594918503E-21</c:v>
+                  <c:v>4.1969394353350485E-21</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.8432310820697546E-20</c:v>
+                  <c:v>1.5129082861073815E-20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.9718840697446029E-20</c:v>
+                  <c:v>5.3286012677063849E-20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4853327821464831E-19</c:v>
+                  <c:v>1.8646678393867047E-19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2169809979176447E-18</c:v>
+                  <c:v>6.5131335098095486E-19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.2481613803067933E-18</c:v>
+                  <c:v>2.273787292557307E-18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4828020480775224E-17</c:v>
+                  <c:v>7.9367777882036805E-18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.1755357183033796E-17</c:v>
+                  <c:v>2.7702556782856345E-17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.8064442677958422E-16</c:v>
+                  <c:v>9.6691904295589479E-17</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.3051148313971422E-16</c:v>
+                  <c:v>3.374883875265451E-16</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.2007017951003823E-15</c:v>
+                  <c:v>1.1779506969532916E-15</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.6812044923271107E-15</c:v>
+                  <c:v>4.1114523996730492E-15</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.6810038484943145E-14</c:v>
+                  <c:v>1.4350379408463327E-14</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.35762294955271E-14</c:v>
+                  <c:v>5.0087746185560261E-14</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.2661313408587094E-13</c:v>
+                  <c:v>1.7482341263423132E-13</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.1399918528514886E-12</c:v>
+                  <c:v>6.1019366756766178E-13</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.9789625356443937E-12</c:v>
+                  <c:v>2.1297851707629252E-12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.3887943864771246E-11</c:v>
+                  <c:v>7.4336806721593663E-12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.8473687062510023E-11</c:v>
+                  <c:v>2.5946094982571976E-11</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.6918979226132137E-10</c:v>
+                  <c:v>9.0560769896536766E-11</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.9053039989421534E-10</c:v>
+                  <c:v>3.1608814543117973E-10</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.0611536224383871E-9</c:v>
+                  <c:v>1.1032560323433728E-9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.1941330303252676E-9</c:v>
+                  <c:v>3.8507419227674793E-9</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.5109991557439981E-8</c:v>
+                  <c:v>1.3440409951135022E-8</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8.7642482194437432E-8</c:v>
+                  <c:v>4.6911640218344654E-8</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.0590232050182997E-7</c:v>
+                  <c:v>1.637377130590834E-7</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.0677040100347979E-6</c:v>
+                  <c:v>5.7150077364668012E-7</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.7266531720787243E-6</c:v>
+                  <c:v>1.9947337004816979E-6</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.3007297654067807E-5</c:v>
+                  <c:v>6.962304723488094E-6</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.5399929762485823E-5</c:v>
+                  <c:v>2.4300831259329983E-5</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.5846132511575464E-4</c:v>
+                  <c:v>8.4818235246470971E-5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5.5308437014784544E-4</c:v>
+                  <c:v>2.9604473005686173E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.9304541362277505E-3</c:v>
+                  <c:v>1.0332976386476591E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.737946999085611E-3</c:v>
+                  <c:v>3.6065631360158333E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.3517745856009614E-2</c:v>
+                  <c:v>1.2588142242434357E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8.2084998623901131E-2</c:v>
+                  <c:v>4.3936933623408669E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.28650479686019825</c:v>
+                  <c:v>0.15335496684493283</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.0000000000000215</c:v>
+                  <c:v>0.53526142851900549</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0000000000000355</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2065,504 +2135,510 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>problem1!$H$16:$H$96</c:f>
+              <c:f>problem1!$H$16:$H$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2500000000000001E-2</c:v>
+                  <c:v>6.2500000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>1.8750000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.7500000000000006E-2</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.05</c:v>
+                  <c:v>4.3749999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>5.6249999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.4999999999999997E-2</c:v>
+                  <c:v>6.8749999999999992E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.7499999999999994E-2</c:v>
+                  <c:v>8.1249999999999989E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.9999999999999992E-2</c:v>
+                  <c:v>9.3749999999999986E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.11249999999999999</c:v>
+                  <c:v>0.10624999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.12499999999999999</c:v>
+                  <c:v>0.11874999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.13749999999999998</c:v>
+                  <c:v>0.13124999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.15</c:v>
+                  <c:v>0.14374999999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.16250000000000001</c:v>
+                  <c:v>0.15625</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.17500000000000002</c:v>
+                  <c:v>0.16875000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.18750000000000003</c:v>
+                  <c:v>0.18125000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.20000000000000004</c:v>
+                  <c:v>0.19375000000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.21250000000000005</c:v>
+                  <c:v>0.20625000000000004</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.22500000000000006</c:v>
+                  <c:v>0.21875000000000006</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.23750000000000007</c:v>
+                  <c:v>0.23125000000000007</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.25000000000000006</c:v>
+                  <c:v>0.24375000000000008</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.26250000000000007</c:v>
+                  <c:v>0.25625000000000009</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.27500000000000008</c:v>
+                  <c:v>0.2687500000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.28750000000000009</c:v>
+                  <c:v>0.28125000000000011</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.3000000000000001</c:v>
+                  <c:v>0.29375000000000012</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.31250000000000011</c:v>
+                  <c:v>0.30625000000000013</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.32500000000000012</c:v>
+                  <c:v>0.31875000000000014</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.33750000000000013</c:v>
+                  <c:v>0.33125000000000016</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.35000000000000014</c:v>
+                  <c:v>0.34375000000000017</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.36250000000000016</c:v>
+                  <c:v>0.35625000000000018</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.37500000000000017</c:v>
+                  <c:v>0.36875000000000019</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.38750000000000018</c:v>
+                  <c:v>0.3812500000000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.40000000000000019</c:v>
+                  <c:v>0.39375000000000021</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.4125000000000002</c:v>
+                  <c:v>0.40625000000000022</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.42500000000000021</c:v>
+                  <c:v>0.41875000000000023</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.43750000000000022</c:v>
+                  <c:v>0.43125000000000024</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.45000000000000023</c:v>
+                  <c:v>0.44375000000000026</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.46250000000000024</c:v>
+                  <c:v>0.45625000000000027</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.47500000000000026</c:v>
+                  <c:v>0.46875000000000028</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.48750000000000027</c:v>
+                  <c:v>0.48125000000000029</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.50000000000000022</c:v>
+                  <c:v>0.4937500000000003</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.51250000000000018</c:v>
+                  <c:v>0.50625000000000031</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.52500000000000013</c:v>
+                  <c:v>0.51875000000000027</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.53750000000000009</c:v>
+                  <c:v>0.53125000000000022</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.54375000000000018</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.5625</c:v>
+                  <c:v>0.55625000000000013</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.57499999999999996</c:v>
+                  <c:v>0.56875000000000009</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.58749999999999991</c:v>
+                  <c:v>0.58125000000000004</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.59999999999999987</c:v>
+                  <c:v>0.59375</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.61249999999999982</c:v>
+                  <c:v>0.60624999999999996</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.62499999999999978</c:v>
+                  <c:v>0.61874999999999991</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.63749999999999973</c:v>
+                  <c:v>0.63124999999999987</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.64999999999999969</c:v>
+                  <c:v>0.64374999999999982</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.66249999999999964</c:v>
+                  <c:v>0.65624999999999978</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.6749999999999996</c:v>
+                  <c:v>0.66874999999999973</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.68749999999999956</c:v>
+                  <c:v>0.68124999999999969</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.69999999999999951</c:v>
+                  <c:v>0.69374999999999964</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.71249999999999947</c:v>
+                  <c:v>0.7062499999999996</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.72499999999999942</c:v>
+                  <c:v>0.71874999999999956</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.73749999999999938</c:v>
+                  <c:v>0.73124999999999951</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.74999999999999933</c:v>
+                  <c:v>0.74374999999999947</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.76249999999999929</c:v>
+                  <c:v>0.75624999999999942</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.77499999999999925</c:v>
+                  <c:v>0.76874999999999938</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.7874999999999992</c:v>
+                  <c:v>0.78124999999999933</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.79999999999999916</c:v>
+                  <c:v>0.79374999999999929</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.81249999999999911</c:v>
+                  <c:v>0.80624999999999925</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.82499999999999907</c:v>
+                  <c:v>0.8187499999999992</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.83749999999999902</c:v>
+                  <c:v>0.83124999999999916</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.84999999999999898</c:v>
+                  <c:v>0.84374999999999911</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.86249999999999893</c:v>
+                  <c:v>0.85624999999999907</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.87499999999999889</c:v>
+                  <c:v>0.86874999999999902</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.88749999999999885</c:v>
+                  <c:v>0.88124999999999898</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.8999999999999988</c:v>
+                  <c:v>0.89374999999999893</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.91249999999999876</c:v>
+                  <c:v>0.90624999999999889</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.92499999999999871</c:v>
+                  <c:v>0.91874999999999885</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.93749999999999867</c:v>
+                  <c:v>0.9312499999999988</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.94999999999999862</c:v>
+                  <c:v>0.94374999999999876</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.96249999999999858</c:v>
+                  <c:v>0.95624999999999871</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.97499999999999853</c:v>
+                  <c:v>0.96874999999999867</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.98749999999999849</c:v>
+                  <c:v>0.98124999999999862</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.99999999999999845</c:v>
+                  <c:v>0.99374999999999858</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.99999999999999856</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>problem1!$I$16:$I$96</c:f>
+              <c:f>problem1!$I$16:$I$97</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="82"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6746292583926853E-22</c:v>
+                  <c:v>7.0753862326635635E-23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8032486005825407E-22</c:v>
+                  <c:v>2.9964854310372168E-22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0648279038972999E-21</c:v>
+                  <c:v>7.2728010514325144E-22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1568233526564253E-21</c:v>
+                  <c:v>1.5262010421940298E-21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.1969394353350485E-21</c:v>
+                  <c:v>3.0187818531471079E-21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0083780594918458E-21</c:v>
+                  <c:v>5.807289919351105E-21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5129082861073815E-20</c:v>
+                  <c:v>1.1016908841303863E-20</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8432310820697546E-20</c:v>
+                  <c:v>2.0749758332004521E-20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.3286012677063849E-20</c:v>
+                  <c:v>3.8933115047302286E-20</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.9718840697445945E-20</c:v>
+                  <c:v>7.2904097723205404E-20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.8646678393867047E-19</c:v>
+                  <c:v>1.3637024877746143E-19</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.4853327821464831E-19</c:v>
+                  <c:v>2.5494062891835805E-19</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.5131335098095601E-19</c:v>
+                  <c:v>4.7645926228779048E-19</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.2169809979176447E-18</c:v>
+                  <c:v>8.9031055357614268E-19</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.2737872925573151E-18</c:v>
+                  <c:v>1.6634865555037151E-18</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.2481613803068002E-18</c:v>
+                  <c:v>3.1079694954885074E-18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.9367777882037098E-18</c:v>
+                  <c:v>5.8066189086949072E-18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.4828020480775301E-17</c:v>
+                  <c:v>1.0848359765444622E-17</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.7702556782856493E-17</c:v>
+                  <c:v>2.0267571739488127E-17</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.1755357183034079E-17</c:v>
+                  <c:v>3.7864976432192083E-17</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.6691904295589997E-17</c:v>
+                  <c:v>7.0741256610635084E-17</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.8064442677958518E-16</c:v>
+                  <c:v>1.3216223414942054E-16</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.3748838752654698E-16</c:v>
+                  <c:v>2.4691172713779154E-16</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>6.3051148313971748E-16</c:v>
+                  <c:v>4.6129200353071282E-16</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.1779506969532979E-15</c:v>
+                  <c:v>8.6180708825499227E-16</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.2007017951003977E-15</c:v>
+                  <c:v>1.6100677761817495E-15</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.1114523996730792E-15</c:v>
+                  <c:v>3.0080027815063676E-15</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.6812044923271659E-15</c:v>
+                  <c:v>5.6196892039570783E-15</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.4350379408463377E-14</c:v>
+                  <c:v>1.049896180478124E-14</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.681003848494324E-14</c:v>
+                  <c:v>1.9614643116480858E-14</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.0087746185560444E-14</c:v>
+                  <c:v>3.6644977876304056E-14</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>9.3576229495527769E-14</c:v>
+                  <c:v>6.8461831945061219E-14</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.7482341263423255E-13</c:v>
+                  <c:v>1.279035409372277E-13</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.2661313408587321E-13</c:v>
+                  <c:v>2.3895527346470535E-13</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.10193667567664E-13</c:v>
+                  <c:v>4.4642722382500994E-13</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.1399918528514926E-12</c:v>
+                  <c:v>8.3403585636623067E-13</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.1297851707629329E-12</c:v>
+                  <c:v>1.5581841171771949E-12</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.9789625356444219E-12</c:v>
+                  <c:v>2.9110711780188537E-12</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>7.4336806721594196E-12</c:v>
+                  <c:v>5.4385969602986439E-12</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.3887943864771296E-11</c:v>
+                  <c:v>1.0160636785348578E-11</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.5946094982571976E-11</c:v>
+                  <c:v>1.8982568599332073E-11</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.8473687062510023E-11</c:v>
+                  <c:v>3.5464107047549455E-11</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>9.0560769896536133E-11</c:v>
+                  <c:v>6.6255674625695089E-11</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.6918979226132078E-10</c:v>
+                  <c:v>1.2378189627656654E-10</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.1608814543117642E-10</c:v>
+                  <c:v>2.3125502732215755E-10</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.9053039989420903E-10</c:v>
+                  <c:v>4.320412699306649E-10</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.1032560323433573E-9</c:v>
+                  <c:v>8.0715935599201584E-10</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.0611536224383507E-9</c:v>
+                  <c:v>1.5079722038358418E-9</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.8507419227673974E-9</c:v>
+                  <c:v>2.817262973736628E-9</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>7.1941330303251137E-9</c:v>
+                  <c:v>5.2633401617071044E-9</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.3440409951134639E-8</c:v>
+                  <c:v>9.8332139797000909E-9</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.5109991557439273E-8</c:v>
+                  <c:v>1.8370862266140877E-8</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.6911640218343317E-8</c:v>
+                  <c:v>3.4321289163261772E-8</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>8.7642482194434308E-8</c:v>
+                  <c:v>6.4120609733126306E-8</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.6373771305907761E-7</c:v>
+                  <c:v>1.1979306992200262E-7</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>3.0590232050181912E-7</c:v>
+                  <c:v>2.238029186101771E-7</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>5.7150077364665566E-7</c:v>
+                  <c:v>4.1811889795499329E-7</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.0677040100347524E-6</c:v>
+                  <c:v>7.8114894083043226E-7</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.9947337004815992E-6</c:v>
+                  <c:v>1.4593783508589176E-6</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>3.7266531720785384E-6</c:v>
+                  <c:v>2.7264777043562575E-6</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>6.9623047234876992E-6</c:v>
+                  <c:v>5.093730949192664E-6</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.300729765406716E-5</c:v>
+                  <c:v>9.5163422540765913E-6</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2.4300831259328428E-5</c:v>
+                  <c:v>1.7778867945719909E-5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4.5399929762482923E-5</c:v>
+                  <c:v>3.3215298167312543E-5</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>8.481823524646555E-5</c:v>
+                  <c:v>6.2054346525987564E-5</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.5846132511574337E-4</c:v>
+                  <c:v>1.1593278203827371E-4</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>2.9604473005684069E-4</c:v>
+                  <c:v>2.1659095137687581E-4</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.530843701478062E-4</c:v>
+                  <c:v>4.0464516932624728E-4</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.0332976386475783E-3</c:v>
+                  <c:v>7.5597670178823332E-4</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.9304541362275996E-3</c:v>
+                  <c:v>1.4123504170288116E-3</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>3.6065631360155258E-3</c:v>
+                  <c:v>2.6386179570917906E-3</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>6.7379469990850845E-3</c:v>
+                  <c:v>4.9295873315447717E-3</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1.2588142242433193E-2</c:v>
+                  <c:v>9.2096816039676163E-3</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>2.3517745856007605E-2</c:v>
+                  <c:v>1.7205950425850405E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>4.393693362340461E-2</c:v>
+                  <c:v>3.214494732687425E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>8.2084998623892971E-2</c:v>
+                  <c:v>6.0054667895304108E-2</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.15335496684491759</c:v>
+                  <c:v>0.11219689052033657</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.28650479686016977</c:v>
+                  <c:v>0.20961138715108443</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.53526142851894853</c:v>
+                  <c:v>0.39160562667677118</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.99999999999992195</c:v>
+                  <c:v>0.73161562894658982</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.99999999999992906</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8288,10 +8364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I96"/>
+  <dimension ref="B1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B13" sqref="B13:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8301,16 +8377,16 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="E2" s="27" t="s">
+      <c r="C2" s="35"/>
+      <c r="E2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
@@ -8319,12 +8395,12 @@
       <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="26"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
@@ -8363,7 +8439,7 @@
         <f>F5-E5+1</f>
         <v>10</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="23">
         <f>$C$6/G5</f>
         <v>0.1</v>
       </c>
@@ -8425,7 +8501,7 @@
       <c r="F8" s="11">
         <v>81</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="24">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
@@ -8478,52 +8554,52 @@
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="29"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="35"/>
     </row>
     <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25" t="s">
+      <c r="C14" s="30"/>
+      <c r="D14" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="23" t="s">
+      <c r="E14" s="47"/>
+      <c r="F14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="23" t="s">
+      <c r="G14" s="30"/>
+      <c r="H14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="24"/>
+      <c r="I14" s="30"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="43" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="43" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="43" t="s">
         <v>15</v>
       </c>
       <c r="H15" s="16" t="s">
@@ -8537,21 +8613,21 @@
       <c r="B16" s="2">
         <v>0</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="44">
         <f>$C$3+(EXP(B16*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
         <v>0</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="44">
         <f>$C$3+(EXP(D16*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
         <v>0</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="44">
         <f>$C$3+(EXP(F16*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
         <v>0</v>
       </c>
@@ -8565,644 +8641,654 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
-        <f t="shared" ref="B17:B26" si="1">B16+$H$5</f>
-        <v>0.1</v>
-      </c>
-      <c r="C17" s="3">
+        <f>B16+H5/2</f>
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="44">
         <f>$C$3+(EXP(B17*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>2.8432310820697546E-20</v>
+        <v>2.1568233526564253E-21</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" ref="D17:D36" si="2">D16+$H$6</f>
-        <v>0.05</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" ref="E17:E36" si="3">$C$3+(EXP(D17*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>2.1568233526564253E-21</v>
+        <f>D16+H6/2</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E17" s="44">
+        <f t="shared" ref="E17:E37" si="1">$C$3+(EXP(D17*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>4.8032486005825407E-22</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" ref="F17:F56" si="4">F16+$H$7</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="G17" s="3">
-        <f t="shared" ref="G17:G56" si="5">$C$3+(EXP(F17*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>4.8032486005825407E-22</v>
+        <f>F16+H7/2</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="G17" s="44">
+        <f t="shared" ref="G17:G57" si="2">$C$3+(EXP(F17*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>1.6746292583926853E-22</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" ref="H17:H48" si="6">H16+$H$8</f>
-        <v>1.2500000000000001E-2</v>
+        <f>H16+$H$8/2</f>
+        <v>6.2500000000000003E-3</v>
       </c>
       <c r="I17" s="3">
-        <f t="shared" ref="I17:I80" si="7">$C$3+(EXP(H17*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>1.6746292583926853E-22</v>
+        <f t="shared" ref="I17:I80" si="3">$C$3+(EXP(H17*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>7.0753862326635635E-23</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
+        <f t="shared" ref="B17:B26" si="4">B17+$H$5</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="C18" s="44">
+        <f t="shared" ref="C18:C24" si="5">$C$3+(EXP(B18*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>3.485332782146486E-19</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" ref="D17:D36" si="6">D17+$H$6</f>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="E18" s="44">
         <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="C18" s="3">
-        <f t="shared" ref="C17:C25" si="8">$C$3+(EXP(B18*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>4.2481613803067933E-18</v>
-      </c>
-      <c r="D18" s="2">
+        <v>8.0083780594918503E-21</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" ref="F17:F56" si="7">F17+$H$7</f>
+        <v>3.7500000000000006E-2</v>
+      </c>
+      <c r="G18" s="44">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="E18" s="3">
+        <v>1.0648279038972999E-21</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" ref="H17:H48" si="8">H17+$H$8</f>
+        <v>1.8750000000000003E-2</v>
+      </c>
+      <c r="I18" s="3">
         <f t="shared" si="3"/>
-        <v>2.8432310820697546E-20</v>
-      </c>
-      <c r="F18" s="2">
-        <f t="shared" si="4"/>
-        <v>0.05</v>
-      </c>
-      <c r="G18" s="3">
-        <f t="shared" si="5"/>
-        <v>2.1568233526564253E-21</v>
-      </c>
-      <c r="H18" s="2">
-        <f t="shared" si="6"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="I18" s="3">
-        <f t="shared" si="7"/>
-        <v>4.8032486005825407E-22</v>
+        <v>2.9964854310372168E-22</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="C19" s="44">
+        <f t="shared" si="5"/>
+        <v>5.1755357183033894E-17</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="6"/>
+        <v>0.125</v>
+      </c>
+      <c r="E19" s="44">
         <f t="shared" si="1"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="C19" s="3">
+        <v>9.9718840697446029E-20</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="7"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="G19" s="44">
+        <f t="shared" si="2"/>
+        <v>4.1969394353350485E-21</v>
+      </c>
+      <c r="H19" s="2">
         <f t="shared" si="8"/>
-        <v>6.3051148313971531E-16</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="2"/>
-        <v>0.15000000000000002</v>
-      </c>
-      <c r="E19" s="3">
+        <v>3.125E-2</v>
+      </c>
+      <c r="I19" s="3">
         <f t="shared" si="3"/>
-        <v>3.485332782146486E-19</v>
-      </c>
-      <c r="F19" s="2">
-        <f t="shared" si="4"/>
-        <v>7.5000000000000011E-2</v>
-      </c>
-      <c r="G19" s="3">
-        <f t="shared" si="5"/>
-        <v>8.0083780594918503E-21</v>
-      </c>
-      <c r="H19" s="2">
-        <f t="shared" si="6"/>
-        <v>3.7500000000000006E-2</v>
-      </c>
-      <c r="I19" s="3">
-        <f t="shared" si="7"/>
-        <v>1.0648279038972999E-21</v>
+        <v>7.2728010514325144E-22</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
+        <f t="shared" si="4"/>
+        <v>0.35</v>
+      </c>
+      <c r="C20" s="44">
+        <f>$C$3+(EXP(B20*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>7.6812044923271107E-15</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="6"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E20" s="44">
         <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="C20" s="3">
-        <f>$C$3+(EXP(B20*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>9.3576229495526771E-14</v>
-      </c>
-      <c r="D20" s="2">
+        <v>1.2169809979176447E-18</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="7"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="G20" s="44">
         <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="E20" s="3">
+        <v>1.5129082861073815E-20</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="8"/>
+        <v>4.3749999999999997E-2</v>
+      </c>
+      <c r="I20" s="3">
         <f t="shared" si="3"/>
-        <v>4.2481613803067933E-18</v>
-      </c>
-      <c r="F20" s="2">
-        <f t="shared" si="4"/>
-        <v>0.1</v>
-      </c>
-      <c r="G20" s="3">
-        <f t="shared" si="5"/>
-        <v>2.8432310820697546E-20</v>
-      </c>
-      <c r="H20" s="2">
-        <f t="shared" si="6"/>
-        <v>0.05</v>
-      </c>
-      <c r="I20" s="3">
-        <f t="shared" si="7"/>
-        <v>2.1568233526564253E-21</v>
+        <v>1.5262010421940298E-21</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
+        <f t="shared" si="4"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="C21" s="44">
+        <f>$C$3+(EXP(B21*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>1.1399918528514765E-12</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="6"/>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="E21" s="44">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="C21" s="3">
-        <f>$C$3+(EXP(B21*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>1.3887943864771149E-11</v>
-      </c>
-      <c r="D21" s="2">
+        <v>1.4828020480775224E-17</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="7"/>
+        <v>0.11249999999999999</v>
+      </c>
+      <c r="G21" s="44">
         <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="E21" s="3">
+        <v>5.3286012677063849E-20</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="8"/>
+        <v>5.6249999999999994E-2</v>
+      </c>
+      <c r="I21" s="3">
         <f t="shared" si="3"/>
-        <v>5.1755357183033894E-17</v>
-      </c>
-      <c r="F21" s="2">
-        <f t="shared" si="4"/>
-        <v>0.125</v>
-      </c>
-      <c r="G21" s="3">
-        <f t="shared" si="5"/>
-        <v>9.9718840697446029E-20</v>
-      </c>
-      <c r="H21" s="2">
-        <f t="shared" si="6"/>
-        <v>6.25E-2</v>
-      </c>
-      <c r="I21" s="3">
-        <f t="shared" si="7"/>
-        <v>4.1969394353350485E-21</v>
+        <v>3.0187818531471079E-21</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
+        <f t="shared" si="4"/>
+        <v>0.54999999999999993</v>
+      </c>
+      <c r="C22" s="44">
+        <f>$C$3+(EXP(B22*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>1.6918979226131959E-10</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="6"/>
+        <v>0.27499999999999997</v>
+      </c>
+      <c r="E22" s="44">
         <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-      <c r="C22" s="3">
-        <f>$C$3+(EXP(B22*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>2.0611536224383651E-9</v>
-      </c>
-      <c r="D22" s="2">
+        <v>1.8064442677958422E-16</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="7"/>
+        <v>0.13749999999999998</v>
+      </c>
+      <c r="G22" s="44">
         <f t="shared" si="2"/>
-        <v>0.3</v>
-      </c>
-      <c r="E22" s="3">
+        <v>1.8646678393867047E-19</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="8"/>
+        <v>6.8749999999999992E-2</v>
+      </c>
+      <c r="I22" s="3">
         <f t="shared" si="3"/>
-        <v>6.3051148313971422E-16</v>
-      </c>
-      <c r="F22" s="2">
-        <f t="shared" si="4"/>
-        <v>0.15</v>
-      </c>
-      <c r="G22" s="3">
-        <f t="shared" si="5"/>
-        <v>3.4853327821464831E-19</v>
-      </c>
-      <c r="H22" s="2">
-        <f t="shared" si="6"/>
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="I22" s="3">
-        <f t="shared" si="7"/>
-        <v>8.0083780594918458E-21</v>
+        <v>5.807289919351105E-21</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="2">
+        <f t="shared" si="4"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="C23" s="44">
+        <f>$C$3+(EXP(B23*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>2.5109991557439448E-8</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="6"/>
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="E23" s="44">
         <f t="shared" si="1"/>
-        <v>0.7</v>
-      </c>
-      <c r="C23" s="3">
-        <f>$C$3+(EXP(B23*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>3.0590232050182563E-7</v>
-      </c>
-      <c r="D23" s="2">
+        <v>2.2007017951003744E-15</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="7"/>
+        <v>0.16249999999999998</v>
+      </c>
+      <c r="G23" s="44">
         <f t="shared" si="2"/>
-        <v>0.35</v>
-      </c>
-      <c r="E23" s="3">
+        <v>6.5131335098095486E-19</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="8"/>
+        <v>8.1249999999999989E-2</v>
+      </c>
+      <c r="I23" s="3">
         <f t="shared" si="3"/>
-        <v>7.6812044923271107E-15</v>
-      </c>
-      <c r="F23" s="2">
-        <f t="shared" si="4"/>
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="G23" s="3">
-        <f t="shared" si="5"/>
-        <v>1.2169809979176447E-18</v>
-      </c>
-      <c r="H23" s="2">
-        <f t="shared" si="6"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="I23" s="3">
-        <f t="shared" si="7"/>
-        <v>1.5129082861073815E-20</v>
+        <v>1.1016908841303863E-20</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
+        <f t="shared" si="4"/>
+        <v>0.74999999999999989</v>
+      </c>
+      <c r="C24" s="44">
+        <f t="shared" si="5"/>
+        <v>3.7266531720786451E-6</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="6"/>
+        <v>0.37499999999999994</v>
+      </c>
+      <c r="E24" s="44">
         <f t="shared" si="1"/>
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="C24" s="3">
+        <v>2.6810038484942956E-14</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="7"/>
+        <v>0.18749999999999997</v>
+      </c>
+      <c r="G24" s="44">
+        <f t="shared" si="2"/>
+        <v>2.273787292557307E-18</v>
+      </c>
+      <c r="H24" s="2">
         <f t="shared" si="8"/>
-        <v>4.5399929762484861E-5</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" si="2"/>
-        <v>0.39999999999999997</v>
-      </c>
-      <c r="E24" s="3">
+        <v>9.3749999999999986E-2</v>
+      </c>
+      <c r="I24" s="3">
         <f t="shared" si="3"/>
-        <v>9.3576229495526771E-14</v>
-      </c>
-      <c r="F24" s="2">
-        <f t="shared" si="4"/>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="G24" s="3">
-        <f t="shared" si="5"/>
-        <v>4.2481613803067933E-18</v>
-      </c>
-      <c r="H24" s="2">
-        <f t="shared" si="6"/>
-        <v>9.9999999999999992E-2</v>
-      </c>
-      <c r="I24" s="3">
-        <f t="shared" si="7"/>
-        <v>2.8432310820697546E-20</v>
+        <v>2.0749758332004521E-20</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
+        <f t="shared" si="4"/>
+        <v>0.84999999999999987</v>
+      </c>
+      <c r="C25" s="44">
+        <f>$C$3+(EXP(B25*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>5.5308437014782972E-4</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="6"/>
+        <v>0.42499999999999993</v>
+      </c>
+      <c r="E25" s="44">
         <f t="shared" si="1"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="C25" s="3">
-        <f>$C$3+(EXP(B25*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>6.7379469990854202E-3</v>
-      </c>
-      <c r="D25" s="2">
+        <v>3.2661313408586857E-13</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="7"/>
+        <v>0.21249999999999997</v>
+      </c>
+      <c r="G25" s="44">
         <f t="shared" si="2"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="E25" s="3">
+        <v>7.9367777882036805E-18</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="8"/>
+        <v>0.10624999999999998</v>
+      </c>
+      <c r="I25" s="3">
         <f t="shared" si="3"/>
-        <v>1.1399918528514765E-12</v>
-      </c>
-      <c r="F25" s="2">
+        <v>3.8933115047302286E-20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B26" s="2">
         <f t="shared" si="4"/>
-        <v>0.22499999999999998</v>
-      </c>
-      <c r="G25" s="3">
-        <f t="shared" si="5"/>
-        <v>1.4828020480775224E-17</v>
-      </c>
-      <c r="H25" s="2">
+        <v>0.94999999999999984</v>
+      </c>
+      <c r="C26" s="44">
+        <f>$C$3+(EXP(B26*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>8.2084998623898217E-2</v>
+      </c>
+      <c r="D26" s="2">
         <f t="shared" si="6"/>
-        <v>0.11249999999999999</v>
-      </c>
-      <c r="I25" s="3">
+        <v>0.47499999999999992</v>
+      </c>
+      <c r="E26" s="44">
+        <f t="shared" si="1"/>
+        <v>3.9789625356443517E-12</v>
+      </c>
+      <c r="F26" s="2">
         <f t="shared" si="7"/>
-        <v>5.3286012677063849E-20</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="4">
+        <v>0.23749999999999996</v>
+      </c>
+      <c r="G26" s="44">
+        <f t="shared" si="2"/>
+        <v>2.7702556782856345E-17</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="8"/>
+        <v>0.11874999999999998</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="3"/>
+        <v>7.2904097723205404E-20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="45">
+        <f>$C$3+(EXP(B27*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="6"/>
+        <v>0.52499999999999991</v>
+      </c>
+      <c r="E27" s="44">
         <f t="shared" si="1"/>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="C26" s="5">
-        <f>$C$3+(EXP(B26*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>0.99999999999999289</v>
-      </c>
-      <c r="D26" s="2">
+        <v>4.8473687062509513E-11</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="7"/>
+        <v>0.26249999999999996</v>
+      </c>
+      <c r="G27" s="44">
         <f t="shared" si="2"/>
-        <v>0.49999999999999994</v>
-      </c>
-      <c r="E26" s="3">
+        <v>9.6691904295589479E-17</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="8"/>
+        <v>0.13124999999999998</v>
+      </c>
+      <c r="I27" s="3">
         <f t="shared" si="3"/>
-        <v>1.3887943864771099E-11</v>
-      </c>
-      <c r="F26" s="2">
-        <f t="shared" si="4"/>
-        <v>0.24999999999999997</v>
-      </c>
-      <c r="G26" s="3">
-        <f t="shared" si="5"/>
-        <v>5.1755357183033796E-17</v>
-      </c>
-      <c r="H26" s="2">
-        <f t="shared" si="6"/>
-        <v>0.12499999999999999</v>
-      </c>
-      <c r="I26" s="3">
-        <f t="shared" si="7"/>
-        <v>9.9718840697445945E-20</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="20"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="2">
-        <f t="shared" si="2"/>
-        <v>0.54999999999999993</v>
-      </c>
-      <c r="E27" s="3">
-        <f t="shared" si="3"/>
-        <v>1.6918979226131959E-10</v>
-      </c>
-      <c r="F27" s="2">
-        <f t="shared" si="4"/>
-        <v>0.27499999999999997</v>
-      </c>
-      <c r="G27" s="3">
-        <f t="shared" si="5"/>
-        <v>1.8064442677958422E-16</v>
-      </c>
-      <c r="H27" s="2">
-        <f t="shared" si="6"/>
-        <v>0.13749999999999998</v>
-      </c>
-      <c r="I27" s="3">
-        <f t="shared" si="7"/>
-        <v>1.8646678393867047E-19</v>
+        <v>1.3637024877746143E-19</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="20"/>
       <c r="C28" s="18"/>
       <c r="D28" s="2">
+        <f t="shared" si="6"/>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="E28" s="44">
+        <f t="shared" si="1"/>
+        <v>5.9053039989420903E-10</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="7"/>
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="G28" s="44">
         <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-      <c r="E28" s="3">
+        <v>3.374883875265451E-16</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="8"/>
+        <v>0.14374999999999999</v>
+      </c>
+      <c r="I28" s="3">
         <f t="shared" si="3"/>
-        <v>2.0611536224383651E-9</v>
-      </c>
-      <c r="F28" s="2">
-        <f t="shared" si="4"/>
-        <v>0.3</v>
-      </c>
-      <c r="G28" s="3">
-        <f t="shared" si="5"/>
-        <v>6.3051148313971422E-16</v>
-      </c>
-      <c r="H28" s="2">
-        <f t="shared" si="6"/>
-        <v>0.15</v>
-      </c>
-      <c r="I28" s="3">
-        <f t="shared" si="7"/>
-        <v>3.4853327821464831E-19</v>
+        <v>2.5494062891835805E-19</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="20"/>
       <c r="C29" s="18"/>
       <c r="D29" s="2">
+        <f t="shared" si="6"/>
+        <v>0.625</v>
+      </c>
+      <c r="E29" s="44">
+        <f t="shared" si="1"/>
+        <v>7.1941330303251907E-9</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="7"/>
+        <v>0.3125</v>
+      </c>
+      <c r="G29" s="44">
         <f t="shared" si="2"/>
-        <v>0.65</v>
-      </c>
-      <c r="E29" s="3">
+        <v>1.1779506969532916E-15</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="8"/>
+        <v>0.15625</v>
+      </c>
+      <c r="I29" s="3">
         <f t="shared" si="3"/>
-        <v>2.5109991557439627E-8</v>
-      </c>
-      <c r="F29" s="2">
-        <f t="shared" si="4"/>
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="G29" s="3">
-        <f t="shared" si="5"/>
-        <v>2.2007017951003823E-15</v>
-      </c>
-      <c r="H29" s="2">
-        <f t="shared" si="6"/>
-        <v>0.16250000000000001</v>
-      </c>
-      <c r="I29" s="3">
-        <f t="shared" si="7"/>
-        <v>6.5131335098095601E-19</v>
+        <v>4.7645926228779048E-19</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="20"/>
       <c r="C30" s="18"/>
       <c r="D30" s="2">
+        <f t="shared" si="6"/>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="E30" s="44">
+        <f t="shared" si="1"/>
+        <v>8.7642482194436174E-8</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="7"/>
+        <v>0.33750000000000002</v>
+      </c>
+      <c r="G30" s="44">
         <f t="shared" si="2"/>
-        <v>0.70000000000000007</v>
-      </c>
-      <c r="E30" s="3">
+        <v>4.1114523996730492E-15</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="8"/>
+        <v>0.16875000000000001</v>
+      </c>
+      <c r="I30" s="3">
         <f t="shared" si="3"/>
-        <v>3.0590232050182563E-7</v>
-      </c>
-      <c r="F30" s="2">
-        <f t="shared" si="4"/>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="G30" s="3">
-        <f t="shared" si="5"/>
-        <v>7.6812044923271107E-15</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" si="6"/>
-        <v>0.17500000000000002</v>
-      </c>
-      <c r="I30" s="3">
-        <f t="shared" si="7"/>
-        <v>1.2169809979176447E-18</v>
+        <v>8.9031055357614268E-19</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="20"/>
       <c r="C31" s="18"/>
       <c r="D31" s="2">
+        <f t="shared" si="6"/>
+        <v>0.72500000000000009</v>
+      </c>
+      <c r="E31" s="44">
+        <f t="shared" si="1"/>
+        <v>1.0677040100347901E-6</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="7"/>
+        <v>0.36250000000000004</v>
+      </c>
+      <c r="G31" s="44">
         <f t="shared" si="2"/>
-        <v>0.75000000000000011</v>
-      </c>
-      <c r="E31" s="3">
+        <v>1.4350379408463327E-14</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="8"/>
+        <v>0.18125000000000002</v>
+      </c>
+      <c r="I31" s="3">
         <f t="shared" si="3"/>
-        <v>3.7266531720786976E-6</v>
-      </c>
-      <c r="F31" s="2">
-        <f t="shared" si="4"/>
-        <v>0.37500000000000006</v>
-      </c>
-      <c r="G31" s="3">
-        <f t="shared" si="5"/>
-        <v>2.6810038484943145E-14</v>
-      </c>
-      <c r="H31" s="2">
-        <f t="shared" si="6"/>
-        <v>0.18750000000000003</v>
-      </c>
-      <c r="I31" s="3">
-        <f t="shared" si="7"/>
-        <v>2.2737872925573151E-18</v>
+        <v>1.6634865555037151E-18</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="20"/>
       <c r="C32" s="18"/>
       <c r="D32" s="2">
+        <f t="shared" si="6"/>
+        <v>0.77500000000000013</v>
+      </c>
+      <c r="E32" s="44">
+        <f t="shared" si="1"/>
+        <v>1.3007297654067714E-5</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="7"/>
+        <v>0.38750000000000007</v>
+      </c>
+      <c r="G32" s="44">
         <f t="shared" si="2"/>
-        <v>0.80000000000000016</v>
-      </c>
-      <c r="E32" s="3">
+        <v>5.0087746185560261E-14</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="8"/>
+        <v>0.19375000000000003</v>
+      </c>
+      <c r="I32" s="3">
         <f t="shared" si="3"/>
-        <v>4.5399929762485179E-5</v>
-      </c>
-      <c r="F32" s="2">
-        <f t="shared" si="4"/>
-        <v>0.40000000000000008</v>
-      </c>
-      <c r="G32" s="3">
-        <f t="shared" si="5"/>
-        <v>9.35762294955271E-14</v>
-      </c>
-      <c r="H32" s="2">
-        <f t="shared" si="6"/>
-        <v>0.20000000000000004</v>
-      </c>
-      <c r="I32" s="3">
-        <f t="shared" si="7"/>
-        <v>4.2481613803068002E-18</v>
+        <v>3.1079694954885074E-18</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="20"/>
       <c r="C33" s="18"/>
       <c r="D33" s="2">
+        <f t="shared" si="6"/>
+        <v>0.82500000000000018</v>
+      </c>
+      <c r="E33" s="44">
+        <f t="shared" si="1"/>
+        <v>1.5846132511575239E-4</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="7"/>
+        <v>0.41250000000000009</v>
+      </c>
+      <c r="G33" s="44">
         <f t="shared" si="2"/>
-        <v>0.8500000000000002</v>
-      </c>
-      <c r="E33" s="3">
+        <v>1.7482341263423132E-13</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="8"/>
+        <v>0.20625000000000004</v>
+      </c>
+      <c r="I33" s="3">
         <f t="shared" si="3"/>
-        <v>5.5308437014783753E-4</v>
-      </c>
-      <c r="F33" s="2">
-        <f t="shared" si="4"/>
-        <v>0.4250000000000001</v>
-      </c>
-      <c r="G33" s="3">
-        <f t="shared" si="5"/>
-        <v>3.2661313408587094E-13</v>
-      </c>
-      <c r="H33" s="2">
-        <f t="shared" si="6"/>
-        <v>0.21250000000000005</v>
-      </c>
-      <c r="I33" s="3">
-        <f t="shared" si="7"/>
-        <v>7.9367777882037098E-18</v>
+        <v>5.8066189086949072E-18</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="20"/>
       <c r="C34" s="18"/>
       <c r="D34" s="2">
+        <f t="shared" si="6"/>
+        <v>0.87500000000000022</v>
+      </c>
+      <c r="E34" s="44">
+        <f t="shared" si="1"/>
+        <v>1.9304541362277371E-3</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="7"/>
+        <v>0.43750000000000011</v>
+      </c>
+      <c r="G34" s="44">
         <f t="shared" si="2"/>
-        <v>0.90000000000000024</v>
-      </c>
-      <c r="E34" s="3">
+        <v>6.1019366756766178E-13</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="8"/>
+        <v>0.21875000000000006</v>
+      </c>
+      <c r="I34" s="3">
         <f t="shared" si="3"/>
-        <v>6.7379469990855633E-3</v>
-      </c>
-      <c r="F34" s="2">
-        <f t="shared" si="4"/>
-        <v>0.45000000000000012</v>
-      </c>
-      <c r="G34" s="3">
-        <f t="shared" si="5"/>
-        <v>1.1399918528514886E-12</v>
-      </c>
-      <c r="H34" s="2">
-        <f t="shared" si="6"/>
-        <v>0.22500000000000006</v>
-      </c>
-      <c r="I34" s="3">
-        <f t="shared" si="7"/>
-        <v>1.4828020480775301E-17</v>
+        <v>1.0848359765444622E-17</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="20"/>
       <c r="C35" s="18"/>
       <c r="D35" s="2">
+        <f t="shared" si="6"/>
+        <v>0.92500000000000027</v>
+      </c>
+      <c r="E35" s="44">
+        <f t="shared" si="1"/>
+        <v>2.3517745856009444E-2</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="7"/>
+        <v>0.46250000000000013</v>
+      </c>
+      <c r="G35" s="44">
         <f t="shared" si="2"/>
-        <v>0.95000000000000029</v>
-      </c>
-      <c r="E35" s="3">
+        <v>2.1297851707629252E-12</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="8"/>
+        <v>0.23125000000000007</v>
+      </c>
+      <c r="I35" s="3">
         <f t="shared" si="3"/>
-        <v>8.2084998623899966E-2</v>
-      </c>
-      <c r="F35" s="2">
-        <f t="shared" si="4"/>
-        <v>0.47500000000000014</v>
-      </c>
-      <c r="G35" s="3">
-        <f t="shared" si="5"/>
-        <v>3.9789625356443937E-12</v>
-      </c>
-      <c r="H35" s="2">
-        <f t="shared" si="6"/>
-        <v>0.23750000000000007</v>
-      </c>
-      <c r="I35" s="3">
-        <f t="shared" si="7"/>
-        <v>2.7702556782856493E-17</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>2.0267571739488127E-17</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="20"/>
       <c r="C36" s="18"/>
-      <c r="D36" s="4">
+      <c r="D36" s="2">
+        <f t="shared" si="6"/>
+        <v>0.97500000000000031</v>
+      </c>
+      <c r="E36" s="44">
+        <f t="shared" si="1"/>
+        <v>0.2865047968601942</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="7"/>
+        <v>0.48750000000000016</v>
+      </c>
+      <c r="G36" s="44">
         <f t="shared" si="2"/>
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="E36" s="5">
+        <v>7.4336806721593663E-12</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="8"/>
+        <v>0.24375000000000008</v>
+      </c>
+      <c r="I36" s="3">
         <f t="shared" si="3"/>
-        <v>1.0000000000000144</v>
-      </c>
-      <c r="F36" s="2">
-        <f t="shared" si="4"/>
-        <v>0.50000000000000011</v>
-      </c>
-      <c r="G36" s="3">
-        <f t="shared" si="5"/>
-        <v>1.3887943864771246E-11</v>
-      </c>
-      <c r="H36" s="2">
-        <f t="shared" si="6"/>
-        <v>0.25000000000000006</v>
-      </c>
-      <c r="I36" s="3">
-        <f t="shared" si="7"/>
-        <v>5.1755357183034079E-17</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+        <v>3.7864976432192083E-17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="20"/>
       <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
+      <c r="D37" s="4">
+        <v>1</v>
+      </c>
+      <c r="E37" s="45">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="F37" s="2">
-        <f t="shared" si="4"/>
-        <v>0.52500000000000013</v>
-      </c>
-      <c r="G37" s="3">
-        <f t="shared" si="5"/>
-        <v>4.8473687062510023E-11</v>
+        <f t="shared" si="7"/>
+        <v>0.51250000000000018</v>
+      </c>
+      <c r="G37" s="44">
+        <f t="shared" si="2"/>
+        <v>2.5946094982571976E-11</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="6"/>
-        <v>0.26250000000000007</v>
+        <f t="shared" si="8"/>
+        <v>0.25625000000000009</v>
       </c>
       <c r="I37" s="3">
-        <f t="shared" si="7"/>
-        <v>9.6691904295589997E-17</v>
+        <f t="shared" si="3"/>
+        <v>7.0741256610635084E-17</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
@@ -9211,20 +9297,20 @@
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
       <c r="F38" s="2">
-        <f t="shared" si="4"/>
-        <v>0.55000000000000016</v>
-      </c>
-      <c r="G38" s="3">
-        <f t="shared" si="5"/>
-        <v>1.6918979226132137E-10</v>
+        <f t="shared" si="7"/>
+        <v>0.5375000000000002</v>
+      </c>
+      <c r="G38" s="44">
+        <f t="shared" si="2"/>
+        <v>9.0560769896536766E-11</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="6"/>
-        <v>0.27500000000000008</v>
+        <f t="shared" si="8"/>
+        <v>0.2687500000000001</v>
       </c>
       <c r="I38" s="3">
-        <f t="shared" si="7"/>
-        <v>1.8064442677958518E-16</v>
+        <f t="shared" si="3"/>
+        <v>1.3216223414942054E-16</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
@@ -9233,20 +9319,20 @@
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
       <c r="F39" s="2">
-        <f t="shared" si="4"/>
-        <v>0.57500000000000018</v>
-      </c>
-      <c r="G39" s="3">
-        <f t="shared" si="5"/>
-        <v>5.9053039989421534E-10</v>
+        <f t="shared" si="7"/>
+        <v>0.56250000000000022</v>
+      </c>
+      <c r="G39" s="44">
+        <f t="shared" si="2"/>
+        <v>3.1608814543117973E-10</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="6"/>
-        <v>0.28750000000000009</v>
+        <f t="shared" si="8"/>
+        <v>0.28125000000000011</v>
       </c>
       <c r="I39" s="3">
-        <f t="shared" si="7"/>
-        <v>3.3748838752654698E-16</v>
+        <f t="shared" si="3"/>
+        <v>2.4691172713779154E-16</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
@@ -9255,20 +9341,20 @@
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
       <c r="F40" s="2">
-        <f t="shared" si="4"/>
-        <v>0.6000000000000002</v>
-      </c>
-      <c r="G40" s="3">
-        <f t="shared" si="5"/>
-        <v>2.0611536224383871E-9</v>
+        <f t="shared" si="7"/>
+        <v>0.58750000000000024</v>
+      </c>
+      <c r="G40" s="44">
+        <f t="shared" si="2"/>
+        <v>1.1032560323433728E-9</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" si="6"/>
-        <v>0.3000000000000001</v>
+        <f t="shared" si="8"/>
+        <v>0.29375000000000012</v>
       </c>
       <c r="I40" s="3">
-        <f t="shared" si="7"/>
-        <v>6.3051148313971748E-16</v>
+        <f t="shared" si="3"/>
+        <v>4.6129200353071282E-16</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
@@ -9277,20 +9363,20 @@
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
       <c r="F41" s="2">
-        <f t="shared" si="4"/>
-        <v>0.62500000000000022</v>
-      </c>
-      <c r="G41" s="3">
-        <f t="shared" si="5"/>
-        <v>7.1941330303252676E-9</v>
+        <f t="shared" si="7"/>
+        <v>0.61250000000000027</v>
+      </c>
+      <c r="G41" s="44">
+        <f t="shared" si="2"/>
+        <v>3.8507419227674793E-9</v>
       </c>
       <c r="H41" s="2">
-        <f t="shared" si="6"/>
-        <v>0.31250000000000011</v>
+        <f t="shared" si="8"/>
+        <v>0.30625000000000013</v>
       </c>
       <c r="I41" s="3">
-        <f t="shared" si="7"/>
-        <v>1.1779506969532979E-15</v>
+        <f t="shared" si="3"/>
+        <v>8.6180708825499227E-16</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
@@ -9299,20 +9385,20 @@
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
       <c r="F42" s="2">
-        <f t="shared" si="4"/>
-        <v>0.65000000000000024</v>
-      </c>
-      <c r="G42" s="3">
-        <f t="shared" si="5"/>
-        <v>2.5109991557439981E-8</v>
+        <f t="shared" si="7"/>
+        <v>0.63750000000000029</v>
+      </c>
+      <c r="G42" s="44">
+        <f t="shared" si="2"/>
+        <v>1.3440409951135022E-8</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" si="6"/>
-        <v>0.32500000000000012</v>
+        <f t="shared" si="8"/>
+        <v>0.31875000000000014</v>
       </c>
       <c r="I42" s="3">
-        <f t="shared" si="7"/>
-        <v>2.2007017951003977E-15</v>
+        <f t="shared" si="3"/>
+        <v>1.6100677761817495E-15</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
@@ -9321,20 +9407,20 @@
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
       <c r="F43" s="2">
-        <f t="shared" si="4"/>
-        <v>0.67500000000000027</v>
-      </c>
-      <c r="G43" s="3">
-        <f t="shared" si="5"/>
-        <v>8.7642482194437432E-8</v>
+        <f t="shared" si="7"/>
+        <v>0.66250000000000031</v>
+      </c>
+      <c r="G43" s="44">
+        <f t="shared" si="2"/>
+        <v>4.6911640218344654E-8</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" si="6"/>
-        <v>0.33750000000000013</v>
+        <f t="shared" si="8"/>
+        <v>0.33125000000000016</v>
       </c>
       <c r="I43" s="3">
-        <f t="shared" si="7"/>
-        <v>4.1114523996730792E-15</v>
+        <f t="shared" si="3"/>
+        <v>3.0080027815063676E-15</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
@@ -9343,20 +9429,20 @@
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
       <c r="F44" s="2">
-        <f t="shared" si="4"/>
-        <v>0.70000000000000029</v>
-      </c>
-      <c r="G44" s="3">
-        <f t="shared" si="5"/>
-        <v>3.0590232050182997E-7</v>
+        <f t="shared" si="7"/>
+        <v>0.68750000000000033</v>
+      </c>
+      <c r="G44" s="44">
+        <f t="shared" si="2"/>
+        <v>1.637377130590834E-7</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" si="6"/>
-        <v>0.35000000000000014</v>
+        <f t="shared" si="8"/>
+        <v>0.34375000000000017</v>
       </c>
       <c r="I44" s="3">
-        <f t="shared" si="7"/>
-        <v>7.6812044923271659E-15</v>
+        <f t="shared" si="3"/>
+        <v>5.6196892039570783E-15</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
@@ -9365,20 +9451,20 @@
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
       <c r="F45" s="2">
-        <f t="shared" si="4"/>
-        <v>0.72500000000000031</v>
-      </c>
-      <c r="G45" s="3">
-        <f t="shared" si="5"/>
-        <v>1.0677040100347979E-6</v>
+        <f t="shared" si="7"/>
+        <v>0.71250000000000036</v>
+      </c>
+      <c r="G45" s="44">
+        <f t="shared" si="2"/>
+        <v>5.7150077364668012E-7</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" si="6"/>
-        <v>0.36250000000000016</v>
+        <f t="shared" si="8"/>
+        <v>0.35625000000000018</v>
       </c>
       <c r="I45" s="3">
-        <f t="shared" si="7"/>
-        <v>1.4350379408463377E-14</v>
+        <f t="shared" si="3"/>
+        <v>1.049896180478124E-14</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
@@ -9387,20 +9473,20 @@
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
       <c r="F46" s="2">
-        <f t="shared" si="4"/>
-        <v>0.75000000000000033</v>
-      </c>
-      <c r="G46" s="3">
-        <f t="shared" si="5"/>
-        <v>3.7266531720787243E-6</v>
+        <f t="shared" si="7"/>
+        <v>0.73750000000000038</v>
+      </c>
+      <c r="G46" s="44">
+        <f t="shared" si="2"/>
+        <v>1.9947337004816979E-6</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" si="6"/>
-        <v>0.37500000000000017</v>
+        <f t="shared" si="8"/>
+        <v>0.36875000000000019</v>
       </c>
       <c r="I46" s="3">
-        <f t="shared" si="7"/>
-        <v>2.681003848494324E-14</v>
+        <f t="shared" si="3"/>
+        <v>1.9614643116480858E-14</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
@@ -9409,20 +9495,20 @@
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
       <c r="F47" s="2">
-        <f t="shared" si="4"/>
-        <v>0.77500000000000036</v>
-      </c>
-      <c r="G47" s="3">
-        <f t="shared" si="5"/>
-        <v>1.3007297654067807E-5</v>
+        <f t="shared" si="7"/>
+        <v>0.7625000000000004</v>
+      </c>
+      <c r="G47" s="44">
+        <f t="shared" si="2"/>
+        <v>6.962304723488094E-6</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" si="6"/>
-        <v>0.38750000000000018</v>
+        <f t="shared" si="8"/>
+        <v>0.3812500000000002</v>
       </c>
       <c r="I47" s="3">
-        <f t="shared" si="7"/>
-        <v>5.0087746185560444E-14</v>
+        <f t="shared" si="3"/>
+        <v>3.6644977876304056E-14</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
@@ -9431,20 +9517,20 @@
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
       <c r="F48" s="2">
-        <f t="shared" si="4"/>
-        <v>0.80000000000000038</v>
-      </c>
-      <c r="G48" s="3">
-        <f t="shared" si="5"/>
-        <v>4.5399929762485823E-5</v>
+        <f t="shared" si="7"/>
+        <v>0.78750000000000042</v>
+      </c>
+      <c r="G48" s="44">
+        <f t="shared" si="2"/>
+        <v>2.4300831259329983E-5</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" si="6"/>
-        <v>0.40000000000000019</v>
+        <f t="shared" si="8"/>
+        <v>0.39375000000000021</v>
       </c>
       <c r="I48" s="3">
-        <f t="shared" si="7"/>
-        <v>9.3576229495527769E-14</v>
+        <f t="shared" si="3"/>
+        <v>6.8461831945061219E-14</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
@@ -9453,20 +9539,20 @@
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
       <c r="F49" s="2">
-        <f t="shared" si="4"/>
-        <v>0.8250000000000004</v>
-      </c>
-      <c r="G49" s="3">
-        <f t="shared" si="5"/>
-        <v>1.5846132511575464E-4</v>
+        <f t="shared" si="7"/>
+        <v>0.81250000000000044</v>
+      </c>
+      <c r="G49" s="44">
+        <f t="shared" si="2"/>
+        <v>8.4818235246470971E-5</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" ref="H49:H80" si="9">H48+$H$8</f>
-        <v>0.4125000000000002</v>
+        <v>0.40625000000000022</v>
       </c>
       <c r="I49" s="3">
-        <f t="shared" si="7"/>
-        <v>1.7482341263423255E-13</v>
+        <f t="shared" si="3"/>
+        <v>1.279035409372277E-13</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
@@ -9475,20 +9561,20 @@
       <c r="D50" s="18"/>
       <c r="E50" s="18"/>
       <c r="F50" s="2">
-        <f t="shared" si="4"/>
-        <v>0.85000000000000042</v>
-      </c>
-      <c r="G50" s="3">
-        <f t="shared" si="5"/>
-        <v>5.5308437014784544E-4</v>
+        <f t="shared" si="7"/>
+        <v>0.83750000000000047</v>
+      </c>
+      <c r="G50" s="44">
+        <f t="shared" si="2"/>
+        <v>2.9604473005686173E-4</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" si="9"/>
-        <v>0.42500000000000021</v>
+        <v>0.41875000000000023</v>
       </c>
       <c r="I50" s="3">
-        <f t="shared" si="7"/>
-        <v>3.2661313408587321E-13</v>
+        <f t="shared" si="3"/>
+        <v>2.3895527346470535E-13</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
@@ -9497,20 +9583,20 @@
       <c r="D51" s="18"/>
       <c r="E51" s="18"/>
       <c r="F51" s="2">
-        <f t="shared" si="4"/>
-        <v>0.87500000000000044</v>
-      </c>
-      <c r="G51" s="3">
-        <f t="shared" si="5"/>
-        <v>1.9304541362277505E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.86250000000000049</v>
+      </c>
+      <c r="G51" s="44">
+        <f t="shared" si="2"/>
+        <v>1.0332976386476591E-3</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" si="9"/>
-        <v>0.43750000000000022</v>
+        <v>0.43125000000000024</v>
       </c>
       <c r="I51" s="3">
-        <f t="shared" si="7"/>
-        <v>6.10193667567664E-13</v>
+        <f t="shared" si="3"/>
+        <v>4.4642722382500994E-13</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
@@ -9519,20 +9605,20 @@
       <c r="D52" s="18"/>
       <c r="E52" s="18"/>
       <c r="F52" s="2">
-        <f t="shared" si="4"/>
-        <v>0.90000000000000047</v>
-      </c>
-      <c r="G52" s="3">
-        <f t="shared" si="5"/>
-        <v>6.737946999085611E-3</v>
+        <f t="shared" si="7"/>
+        <v>0.88750000000000051</v>
+      </c>
+      <c r="G52" s="44">
+        <f t="shared" si="2"/>
+        <v>3.6065631360158333E-3</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" si="9"/>
-        <v>0.45000000000000023</v>
+        <v>0.44375000000000026</v>
       </c>
       <c r="I52" s="3">
-        <f t="shared" si="7"/>
-        <v>1.1399918528514926E-12</v>
+        <f t="shared" si="3"/>
+        <v>8.3403585636623067E-13</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
@@ -9541,20 +9627,20 @@
       <c r="D53" s="18"/>
       <c r="E53" s="18"/>
       <c r="F53" s="2">
-        <f t="shared" si="4"/>
-        <v>0.92500000000000049</v>
-      </c>
-      <c r="G53" s="3">
-        <f t="shared" si="5"/>
-        <v>2.3517745856009614E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.91250000000000053</v>
+      </c>
+      <c r="G53" s="44">
+        <f t="shared" si="2"/>
+        <v>1.2588142242434357E-2</v>
       </c>
       <c r="H53" s="2">
         <f t="shared" si="9"/>
-        <v>0.46250000000000024</v>
+        <v>0.45625000000000027</v>
       </c>
       <c r="I53" s="3">
-        <f t="shared" si="7"/>
-        <v>2.1297851707629329E-12</v>
+        <f t="shared" si="3"/>
+        <v>1.5581841171771949E-12</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
@@ -9563,20 +9649,20 @@
       <c r="D54" s="18"/>
       <c r="E54" s="18"/>
       <c r="F54" s="2">
-        <f t="shared" si="4"/>
-        <v>0.95000000000000051</v>
-      </c>
-      <c r="G54" s="3">
-        <f t="shared" si="5"/>
-        <v>8.2084998623901131E-2</v>
+        <f t="shared" si="7"/>
+        <v>0.93750000000000056</v>
+      </c>
+      <c r="G54" s="44">
+        <f t="shared" si="2"/>
+        <v>4.3936933623408669E-2</v>
       </c>
       <c r="H54" s="2">
         <f t="shared" si="9"/>
-        <v>0.47500000000000026</v>
+        <v>0.46875000000000028</v>
       </c>
       <c r="I54" s="3">
-        <f t="shared" si="7"/>
-        <v>3.9789625356444219E-12</v>
+        <f t="shared" si="3"/>
+        <v>2.9110711780188537E-12</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
@@ -9585,58 +9671,64 @@
       <c r="D55" s="18"/>
       <c r="E55" s="18"/>
       <c r="F55" s="2">
-        <f t="shared" si="4"/>
-        <v>0.97500000000000053</v>
-      </c>
-      <c r="G55" s="3">
-        <f t="shared" si="5"/>
-        <v>0.28650479686019825</v>
+        <f t="shared" si="7"/>
+        <v>0.96250000000000058</v>
+      </c>
+      <c r="G55" s="44">
+        <f t="shared" si="2"/>
+        <v>0.15335496684493283</v>
       </c>
       <c r="H55" s="2">
         <f t="shared" si="9"/>
-        <v>0.48750000000000027</v>
+        <v>0.48125000000000029</v>
       </c>
       <c r="I55" s="3">
-        <f t="shared" si="7"/>
-        <v>7.4336806721594196E-12</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>5.4385969602986439E-12</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="20"/>
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
       <c r="E56" s="18"/>
-      <c r="F56" s="4">
-        <f t="shared" si="4"/>
-        <v>1.0000000000000004</v>
-      </c>
-      <c r="G56" s="5">
-        <f t="shared" si="5"/>
-        <v>1.0000000000000215</v>
+      <c r="F56" s="2">
+        <f t="shared" si="7"/>
+        <v>0.9875000000000006</v>
+      </c>
+      <c r="G56" s="44">
+        <f t="shared" si="2"/>
+        <v>0.53526142851900549</v>
       </c>
       <c r="H56" s="2">
         <f t="shared" si="9"/>
-        <v>0.50000000000000022</v>
+        <v>0.4937500000000003</v>
       </c>
       <c r="I56" s="3">
-        <f t="shared" si="7"/>
-        <v>1.3887943864771296E-11</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>1.0160636785348578E-11</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B57" s="20"/>
       <c r="C57" s="18"/>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
+      <c r="F57" s="48">
+        <f>F56+H7/2</f>
+        <v>1.0000000000000007</v>
+      </c>
+      <c r="G57" s="49">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000355</v>
+      </c>
       <c r="H57" s="2">
         <f t="shared" si="9"/>
-        <v>0.51250000000000018</v>
+        <v>0.50625000000000031</v>
       </c>
       <c r="I57" s="3">
-        <f t="shared" si="7"/>
-        <v>2.5946094982571976E-11</v>
+        <f t="shared" si="3"/>
+        <v>1.8982568599332073E-11</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
@@ -9648,11 +9740,11 @@
       <c r="G58" s="18"/>
       <c r="H58" s="2">
         <f t="shared" si="9"/>
-        <v>0.52500000000000013</v>
+        <v>0.51875000000000027</v>
       </c>
       <c r="I58" s="3">
-        <f t="shared" si="7"/>
-        <v>4.8473687062510023E-11</v>
+        <f t="shared" si="3"/>
+        <v>3.5464107047549455E-11</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
@@ -9664,11 +9756,11 @@
       <c r="G59" s="18"/>
       <c r="H59" s="2">
         <f t="shared" si="9"/>
-        <v>0.53750000000000009</v>
+        <v>0.53125000000000022</v>
       </c>
       <c r="I59" s="3">
-        <f t="shared" si="7"/>
-        <v>9.0560769896536133E-11</v>
+        <f t="shared" si="3"/>
+        <v>6.6255674625695089E-11</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
@@ -9680,11 +9772,11 @@
       <c r="G60" s="18"/>
       <c r="H60" s="2">
         <f t="shared" si="9"/>
-        <v>0.55000000000000004</v>
+        <v>0.54375000000000018</v>
       </c>
       <c r="I60" s="3">
-        <f t="shared" si="7"/>
-        <v>1.6918979226132078E-10</v>
+        <f t="shared" si="3"/>
+        <v>1.2378189627656654E-10</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
@@ -9696,11 +9788,11 @@
       <c r="G61" s="18"/>
       <c r="H61" s="2">
         <f t="shared" si="9"/>
-        <v>0.5625</v>
+        <v>0.55625000000000013</v>
       </c>
       <c r="I61" s="3">
-        <f t="shared" si="7"/>
-        <v>3.1608814543117642E-10</v>
+        <f t="shared" si="3"/>
+        <v>2.3125502732215755E-10</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
@@ -9712,11 +9804,11 @@
       <c r="G62" s="18"/>
       <c r="H62" s="2">
         <f t="shared" si="9"/>
-        <v>0.57499999999999996</v>
+        <v>0.56875000000000009</v>
       </c>
       <c r="I62" s="3">
-        <f t="shared" si="7"/>
-        <v>5.9053039989420903E-10</v>
+        <f t="shared" si="3"/>
+        <v>4.320412699306649E-10</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.3">
@@ -9728,11 +9820,11 @@
       <c r="G63" s="18"/>
       <c r="H63" s="2">
         <f t="shared" si="9"/>
-        <v>0.58749999999999991</v>
+        <v>0.58125000000000004</v>
       </c>
       <c r="I63" s="3">
-        <f t="shared" si="7"/>
-        <v>1.1032560323433573E-9</v>
+        <f t="shared" si="3"/>
+        <v>8.0715935599201584E-10</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
@@ -9744,11 +9836,11 @@
       <c r="G64" s="18"/>
       <c r="H64" s="2">
         <f t="shared" si="9"/>
-        <v>0.59999999999999987</v>
+        <v>0.59375</v>
       </c>
       <c r="I64" s="3">
-        <f t="shared" si="7"/>
-        <v>2.0611536224383507E-9</v>
+        <f t="shared" si="3"/>
+        <v>1.5079722038358418E-9</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
@@ -9760,11 +9852,11 @@
       <c r="G65" s="18"/>
       <c r="H65" s="2">
         <f t="shared" si="9"/>
-        <v>0.61249999999999982</v>
+        <v>0.60624999999999996</v>
       </c>
       <c r="I65" s="3">
-        <f t="shared" si="7"/>
-        <v>3.8507419227673974E-9</v>
+        <f t="shared" si="3"/>
+        <v>2.817262973736628E-9</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
@@ -9776,11 +9868,11 @@
       <c r="G66" s="18"/>
       <c r="H66" s="2">
         <f t="shared" si="9"/>
-        <v>0.62499999999999978</v>
+        <v>0.61874999999999991</v>
       </c>
       <c r="I66" s="3">
-        <f t="shared" si="7"/>
-        <v>7.1941330303251137E-9</v>
+        <f t="shared" si="3"/>
+        <v>5.2633401617071044E-9</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
@@ -9792,11 +9884,11 @@
       <c r="G67" s="18"/>
       <c r="H67" s="2">
         <f t="shared" si="9"/>
-        <v>0.63749999999999973</v>
+        <v>0.63124999999999987</v>
       </c>
       <c r="I67" s="3">
-        <f t="shared" si="7"/>
-        <v>1.3440409951134639E-8</v>
+        <f t="shared" si="3"/>
+        <v>9.8332139797000909E-9</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
@@ -9808,11 +9900,11 @@
       <c r="G68" s="18"/>
       <c r="H68" s="2">
         <f t="shared" si="9"/>
-        <v>0.64999999999999969</v>
+        <v>0.64374999999999982</v>
       </c>
       <c r="I68" s="3">
-        <f t="shared" si="7"/>
-        <v>2.5109991557439273E-8</v>
+        <f t="shared" si="3"/>
+        <v>1.8370862266140877E-8</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
@@ -9824,11 +9916,11 @@
       <c r="G69" s="18"/>
       <c r="H69" s="2">
         <f t="shared" si="9"/>
-        <v>0.66249999999999964</v>
+        <v>0.65624999999999978</v>
       </c>
       <c r="I69" s="3">
-        <f t="shared" si="7"/>
-        <v>4.6911640218343317E-8</v>
+        <f t="shared" si="3"/>
+        <v>3.4321289163261772E-8</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
@@ -9840,11 +9932,11 @@
       <c r="G70" s="18"/>
       <c r="H70" s="2">
         <f t="shared" si="9"/>
-        <v>0.6749999999999996</v>
+        <v>0.66874999999999973</v>
       </c>
       <c r="I70" s="3">
-        <f t="shared" si="7"/>
-        <v>8.7642482194434308E-8</v>
+        <f t="shared" si="3"/>
+        <v>6.4120609733126306E-8</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.3">
@@ -9856,11 +9948,11 @@
       <c r="G71" s="18"/>
       <c r="H71" s="2">
         <f t="shared" si="9"/>
-        <v>0.68749999999999956</v>
+        <v>0.68124999999999969</v>
       </c>
       <c r="I71" s="3">
-        <f t="shared" si="7"/>
-        <v>1.6373771305907761E-7</v>
+        <f t="shared" si="3"/>
+        <v>1.1979306992200262E-7</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
@@ -9872,11 +9964,11 @@
       <c r="G72" s="18"/>
       <c r="H72" s="2">
         <f t="shared" si="9"/>
-        <v>0.69999999999999951</v>
+        <v>0.69374999999999964</v>
       </c>
       <c r="I72" s="3">
-        <f t="shared" si="7"/>
-        <v>3.0590232050181912E-7</v>
+        <f t="shared" si="3"/>
+        <v>2.238029186101771E-7</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.3">
@@ -9888,11 +9980,11 @@
       <c r="G73" s="18"/>
       <c r="H73" s="2">
         <f t="shared" si="9"/>
-        <v>0.71249999999999947</v>
+        <v>0.7062499999999996</v>
       </c>
       <c r="I73" s="3">
-        <f t="shared" si="7"/>
-        <v>5.7150077364665566E-7</v>
+        <f t="shared" si="3"/>
+        <v>4.1811889795499329E-7</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
@@ -9904,11 +9996,11 @@
       <c r="G74" s="18"/>
       <c r="H74" s="2">
         <f t="shared" si="9"/>
-        <v>0.72499999999999942</v>
+        <v>0.71874999999999956</v>
       </c>
       <c r="I74" s="3">
-        <f t="shared" si="7"/>
-        <v>1.0677040100347524E-6</v>
+        <f t="shared" si="3"/>
+        <v>7.8114894083043226E-7</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.3">
@@ -9920,11 +10012,11 @@
       <c r="G75" s="18"/>
       <c r="H75" s="2">
         <f t="shared" si="9"/>
-        <v>0.73749999999999938</v>
+        <v>0.73124999999999951</v>
       </c>
       <c r="I75" s="3">
-        <f t="shared" si="7"/>
-        <v>1.9947337004815992E-6</v>
+        <f t="shared" si="3"/>
+        <v>1.4593783508589176E-6</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
@@ -9936,11 +10028,11 @@
       <c r="G76" s="18"/>
       <c r="H76" s="2">
         <f t="shared" si="9"/>
-        <v>0.74999999999999933</v>
+        <v>0.74374999999999947</v>
       </c>
       <c r="I76" s="3">
-        <f t="shared" si="7"/>
-        <v>3.7266531720785384E-6</v>
+        <f t="shared" si="3"/>
+        <v>2.7264777043562575E-6</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.3">
@@ -9952,11 +10044,11 @@
       <c r="G77" s="18"/>
       <c r="H77" s="2">
         <f t="shared" si="9"/>
-        <v>0.76249999999999929</v>
+        <v>0.75624999999999942</v>
       </c>
       <c r="I77" s="3">
-        <f t="shared" si="7"/>
-        <v>6.9623047234876992E-6</v>
+        <f t="shared" si="3"/>
+        <v>5.093730949192664E-6</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.3">
@@ -9968,11 +10060,11 @@
       <c r="G78" s="18"/>
       <c r="H78" s="2">
         <f t="shared" si="9"/>
-        <v>0.77499999999999925</v>
+        <v>0.76874999999999938</v>
       </c>
       <c r="I78" s="3">
-        <f t="shared" si="7"/>
-        <v>1.300729765406716E-5</v>
+        <f t="shared" si="3"/>
+        <v>9.5163422540765913E-6</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
@@ -9984,11 +10076,11 @@
       <c r="G79" s="18"/>
       <c r="H79" s="2">
         <f t="shared" si="9"/>
-        <v>0.7874999999999992</v>
+        <v>0.78124999999999933</v>
       </c>
       <c r="I79" s="3">
-        <f t="shared" si="7"/>
-        <v>2.4300831259328428E-5</v>
+        <f t="shared" si="3"/>
+        <v>1.7778867945719909E-5</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.3">
@@ -10000,11 +10092,11 @@
       <c r="G80" s="18"/>
       <c r="H80" s="2">
         <f t="shared" si="9"/>
-        <v>0.79999999999999916</v>
+        <v>0.79374999999999929</v>
       </c>
       <c r="I80" s="3">
-        <f t="shared" si="7"/>
-        <v>4.5399929762482923E-5</v>
+        <f t="shared" si="3"/>
+        <v>3.3215298167312543E-5</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.3">
@@ -10015,12 +10107,12 @@
       <c r="F81" s="18"/>
       <c r="G81" s="18"/>
       <c r="H81" s="2">
-        <f t="shared" ref="H81:H96" si="10">H80+$H$8</f>
-        <v>0.81249999999999911</v>
+        <f t="shared" ref="H81:H97" si="10">H80+$H$8</f>
+        <v>0.80624999999999925</v>
       </c>
       <c r="I81" s="3">
-        <f t="shared" ref="I81:I96" si="11">$C$3+(EXP(H81*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
-        <v>8.481823524646555E-5</v>
+        <f t="shared" ref="I81:I97" si="11">$C$3+(EXP(H81*$C$5/$C$6)-1)/(EXP($C$5)-1)*($C$4-$C$3)</f>
+        <v>6.2054346525987564E-5</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.3">
@@ -10032,11 +10124,11 @@
       <c r="G82" s="18"/>
       <c r="H82" s="2">
         <f t="shared" si="10"/>
-        <v>0.82499999999999907</v>
+        <v>0.8187499999999992</v>
       </c>
       <c r="I82" s="3">
         <f t="shared" si="11"/>
-        <v>1.5846132511574337E-4</v>
+        <v>1.1593278203827371E-4</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.3">
@@ -10048,11 +10140,11 @@
       <c r="G83" s="18"/>
       <c r="H83" s="2">
         <f t="shared" si="10"/>
-        <v>0.83749999999999902</v>
+        <v>0.83124999999999916</v>
       </c>
       <c r="I83" s="3">
         <f t="shared" si="11"/>
-        <v>2.9604473005684069E-4</v>
+        <v>2.1659095137687581E-4</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.3">
@@ -10064,11 +10156,11 @@
       <c r="G84" s="18"/>
       <c r="H84" s="2">
         <f t="shared" si="10"/>
-        <v>0.84999999999999898</v>
+        <v>0.84374999999999911</v>
       </c>
       <c r="I84" s="3">
         <f t="shared" si="11"/>
-        <v>5.530843701478062E-4</v>
+        <v>4.0464516932624728E-4</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.3">
@@ -10080,11 +10172,11 @@
       <c r="G85" s="18"/>
       <c r="H85" s="2">
         <f t="shared" si="10"/>
-        <v>0.86249999999999893</v>
+        <v>0.85624999999999907</v>
       </c>
       <c r="I85" s="3">
         <f t="shared" si="11"/>
-        <v>1.0332976386475783E-3</v>
+        <v>7.5597670178823332E-4</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.3">
@@ -10096,11 +10188,11 @@
       <c r="G86" s="18"/>
       <c r="H86" s="2">
         <f t="shared" si="10"/>
-        <v>0.87499999999999889</v>
+        <v>0.86874999999999902</v>
       </c>
       <c r="I86" s="3">
         <f t="shared" si="11"/>
-        <v>1.9304541362275996E-3</v>
+        <v>1.4123504170288116E-3</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
@@ -10112,11 +10204,11 @@
       <c r="G87" s="18"/>
       <c r="H87" s="2">
         <f t="shared" si="10"/>
-        <v>0.88749999999999885</v>
+        <v>0.88124999999999898</v>
       </c>
       <c r="I87" s="3">
         <f t="shared" si="11"/>
-        <v>3.6065631360155258E-3</v>
+        <v>2.6386179570917906E-3</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.3">
@@ -10128,11 +10220,11 @@
       <c r="G88" s="18"/>
       <c r="H88" s="2">
         <f t="shared" si="10"/>
-        <v>0.8999999999999988</v>
+        <v>0.89374999999999893</v>
       </c>
       <c r="I88" s="3">
         <f t="shared" si="11"/>
-        <v>6.7379469990850845E-3</v>
+        <v>4.9295873315447717E-3</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.3">
@@ -10144,11 +10236,11 @@
       <c r="G89" s="18"/>
       <c r="H89" s="2">
         <f t="shared" si="10"/>
-        <v>0.91249999999999876</v>
+        <v>0.90624999999999889</v>
       </c>
       <c r="I89" s="3">
         <f t="shared" si="11"/>
-        <v>1.2588142242433193E-2</v>
+        <v>9.2096816039676163E-3</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.3">
@@ -10160,11 +10252,11 @@
       <c r="G90" s="18"/>
       <c r="H90" s="2">
         <f t="shared" si="10"/>
-        <v>0.92499999999999871</v>
+        <v>0.91874999999999885</v>
       </c>
       <c r="I90" s="3">
         <f t="shared" si="11"/>
-        <v>2.3517745856007605E-2</v>
+        <v>1.7205950425850405E-2</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.3">
@@ -10176,11 +10268,11 @@
       <c r="G91" s="18"/>
       <c r="H91" s="2">
         <f t="shared" si="10"/>
-        <v>0.93749999999999867</v>
+        <v>0.9312499999999988</v>
       </c>
       <c r="I91" s="3">
         <f t="shared" si="11"/>
-        <v>4.393693362340461E-2</v>
+        <v>3.214494732687425E-2</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
@@ -10192,11 +10284,11 @@
       <c r="G92" s="18"/>
       <c r="H92" s="2">
         <f t="shared" si="10"/>
-        <v>0.94999999999999862</v>
+        <v>0.94374999999999876</v>
       </c>
       <c r="I92" s="3">
         <f t="shared" si="11"/>
-        <v>8.2084998623892971E-2</v>
+        <v>6.0054667895304108E-2</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.3">
@@ -10208,11 +10300,11 @@
       <c r="G93" s="18"/>
       <c r="H93" s="2">
         <f t="shared" si="10"/>
-        <v>0.96249999999999858</v>
+        <v>0.95624999999999871</v>
       </c>
       <c r="I93" s="3">
         <f t="shared" si="11"/>
-        <v>0.15335496684491759</v>
+        <v>0.11219689052033657</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
@@ -10224,11 +10316,11 @@
       <c r="G94" s="18"/>
       <c r="H94" s="2">
         <f t="shared" si="10"/>
-        <v>0.97499999999999853</v>
+        <v>0.96874999999999867</v>
       </c>
       <c r="I94" s="3">
         <f t="shared" si="11"/>
-        <v>0.28650479686016977</v>
+        <v>0.20961138715108443</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.3">
@@ -10240,27 +10332,43 @@
       <c r="G95" s="18"/>
       <c r="H95" s="2">
         <f t="shared" si="10"/>
-        <v>0.98749999999999849</v>
+        <v>0.98124999999999862</v>
       </c>
       <c r="I95" s="3">
         <f t="shared" si="11"/>
-        <v>0.53526142851894853</v>
-      </c>
-    </row>
-    <row r="96" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B96" s="21"/>
-      <c r="C96" s="22"/>
-      <c r="D96" s="22"/>
-      <c r="E96" s="22"/>
-      <c r="F96" s="22"/>
-      <c r="G96" s="22"/>
-      <c r="H96" s="4">
+        <v>0.39160562667677118</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B96" s="20"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18"/>
+      <c r="H96" s="2">
         <f t="shared" si="10"/>
-        <v>0.99999999999999845</v>
-      </c>
-      <c r="I96" s="5">
+        <v>0.99374999999999858</v>
+      </c>
+      <c r="I96" s="3">
         <f t="shared" si="11"/>
-        <v>0.99999999999992195</v>
+        <v>0.73161562894658982</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B97" s="21"/>
+      <c r="C97" s="22"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="22"/>
+      <c r="F97" s="22"/>
+      <c r="G97" s="22"/>
+      <c r="H97" s="4">
+        <f>H96+$H$8/2</f>
+        <v>0.99999999999999856</v>
+      </c>
+      <c r="I97" s="5">
+        <f t="shared" si="11"/>
+        <v>0.99999999999992906</v>
       </c>
     </row>
   </sheetData>
@@ -10295,16 +10403,16 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="E2" s="27" t="s">
+      <c r="C2" s="35"/>
+      <c r="E2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
@@ -10313,12 +10421,12 @@
       <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="26"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
@@ -10357,7 +10465,7 @@
         <f>F5-E5+1</f>
         <v>5</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="23">
         <f>$C$6/G5</f>
         <v>1</v>
       </c>
@@ -10419,7 +10527,7 @@
       <c r="F8" s="11">
         <v>41</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="24">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -10443,10 +10551,10 @@
       <c r="C10" s="3">
         <v>0.59</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7" t="s">
@@ -10455,10 +10563,10 @@
       <c r="C11" s="3">
         <v>4189</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="39"/>
+      <c r="F11" s="42"/>
     </row>
     <row r="12" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
@@ -10470,7 +10578,7 @@
       <c r="E12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="27" t="s">
         <v>34</v>
       </c>
     </row>
@@ -10481,10 +10589,10 @@
       <c r="C13" s="3">
         <v>1.5</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="25">
         <v>0</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F13" s="26">
         <f>$C$15-($C$15-$C$12)*EXP(-$C$14*$C$16*E13/$C$17/$C$11)</f>
         <v>0</v>
       </c>
@@ -10567,13 +10675,13 @@
     </row>
     <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="41"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E21" s="42">
+      <c r="E21" s="28">
         <f>0</f>
         <v>0</v>
       </c>
@@ -10684,13 +10792,13 @@
     </row>
     <row r="32" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="33" spans="5:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E33" s="40" t="s">
+      <c r="E33" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="38"/>
     </row>
     <row r="34" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E34" s="42">
+      <c r="E34" s="28">
         <v>0</v>
       </c>
       <c r="F34" s="1">
@@ -10710,7 +10818,7 @@
     </row>
     <row r="36" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E36" s="2">
-        <f t="shared" ref="E36:E60" si="6">E35+$H$7</f>
+        <f t="shared" ref="E36:E54" si="6">E35+$H$7</f>
         <v>0.5</v>
       </c>
       <c r="F36" s="3">

</xml_diff>

<commit_message>
assignment 3 changes for dcce
</commit_message>
<xml_diff>
--- a/assignment_3/assignment_3.xlsx
+++ b/assignment_3/assignment_3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="problem1" sheetId="1" r:id="rId1"/>
@@ -1258,66 +1258,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1367,24 +1307,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1442,6 +1364,84 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -12556,8 +12556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AH100"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2:AH8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12568,261 +12568,261 @@
   <sheetData>
     <row r="1" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:34" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="80"/>
-      <c r="S2" s="98" t="s">
+      <c r="C2" s="108"/>
+      <c r="D2" s="109"/>
+      <c r="S2" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="99"/>
-      <c r="U2" s="99"/>
-      <c r="V2" s="100"/>
-      <c r="AE2" s="78" t="s">
+      <c r="T2" s="114"/>
+      <c r="U2" s="114"/>
+      <c r="V2" s="115"/>
+      <c r="AE2" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="AF2" s="79"/>
-      <c r="AG2" s="79"/>
-      <c r="AH2" s="80"/>
+      <c r="AF2" s="108"/>
+      <c r="AG2" s="108"/>
+      <c r="AH2" s="109"/>
     </row>
     <row r="3" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="82">
+      <c r="C3" s="62">
         <v>0</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="S3" s="101" t="s">
+      <c r="S3" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="T3" s="102"/>
-      <c r="U3" s="102"/>
-      <c r="V3" s="103"/>
-      <c r="AE3" s="113" t="s">
+      <c r="T3" s="111"/>
+      <c r="U3" s="111"/>
+      <c r="V3" s="112"/>
+      <c r="AE3" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="AF3" s="109" t="s">
+      <c r="AF3" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="AG3" s="108" t="s">
+      <c r="AG3" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="AH3" s="105" t="s">
+      <c r="AH3" s="79" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="85">
+      <c r="C4" s="65">
         <v>1</v>
       </c>
-      <c r="D4" s="86" t="s">
+      <c r="D4" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="S4" s="104" t="s">
+      <c r="S4" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="T4" s="105" t="s">
+      <c r="T4" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="U4" s="104" t="s">
+      <c r="U4" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="V4" s="105" t="s">
+      <c r="V4" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="AE4" s="114" t="s">
+      <c r="AE4" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="AF4" s="110">
+      <c r="AF4" s="84">
         <v>0</v>
       </c>
-      <c r="AG4" s="90">
+      <c r="AG4" s="70">
         <v>0</v>
       </c>
-      <c r="AH4" s="106" t="s">
+      <c r="AH4" s="80" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="2:34" ht="18" x14ac:dyDescent="0.4">
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="82">
+      <c r="C5" s="62">
         <v>0</v>
       </c>
-      <c r="D5" s="83" t="s">
+      <c r="D5" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="S5" s="89">
+      <c r="S5" s="69">
         <v>2</v>
       </c>
-      <c r="T5" s="106">
+      <c r="T5" s="80">
         <v>11</v>
       </c>
-      <c r="U5" s="81">
+      <c r="U5" s="61">
         <f>T5-S5+1</f>
         <v>10</v>
       </c>
-      <c r="V5" s="83">
+      <c r="V5" s="63">
         <f>$C$7/U5</f>
         <v>0.1</v>
       </c>
-      <c r="AE5" s="115" t="s">
+      <c r="AE5" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="AF5" s="111">
+      <c r="AF5" s="85">
         <v>0</v>
       </c>
-      <c r="AG5" s="92">
+      <c r="AG5" s="72">
         <v>0</v>
       </c>
-      <c r="AH5" s="93" t="s">
+      <c r="AH5" s="73" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="85">
+      <c r="C6" s="65">
         <v>1</v>
       </c>
-      <c r="D6" s="88" t="s">
+      <c r="D6" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="S6" s="94">
+      <c r="S6" s="74">
         <v>2</v>
       </c>
-      <c r="T6" s="93">
+      <c r="T6" s="73">
         <v>21</v>
       </c>
-      <c r="U6" s="89">
+      <c r="U6" s="69">
         <f t="shared" ref="U6:U8" si="0">T6-S6+1</f>
         <v>20</v>
       </c>
-      <c r="V6" s="93">
+      <c r="V6" s="73">
         <f>$C$7/U6</f>
         <v>0.05</v>
       </c>
-      <c r="AE6" s="115" t="s">
+      <c r="AE6" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="AF6" s="111">
+      <c r="AF6" s="85">
         <v>1</v>
       </c>
-      <c r="AG6" s="92">
+      <c r="AG6" s="72">
         <v>1</v>
       </c>
-      <c r="AH6" s="93" t="s">
+      <c r="AH6" s="73" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:34" ht="18" x14ac:dyDescent="0.4">
-      <c r="B7" s="89" t="s">
+      <c r="B7" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="90">
+      <c r="C7" s="70">
         <v>1</v>
       </c>
-      <c r="D7" s="91" t="s">
+      <c r="D7" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="S7" s="94">
+      <c r="S7" s="74">
         <v>2</v>
       </c>
-      <c r="T7" s="93">
+      <c r="T7" s="73">
         <v>41</v>
       </c>
-      <c r="U7" s="89">
+      <c r="U7" s="69">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="V7" s="93">
+      <c r="V7" s="73">
         <f>$C$7/U7</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AE7" s="115" t="s">
+      <c r="AE7" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="AF7" s="111">
+      <c r="AF7" s="85">
         <v>0</v>
       </c>
-      <c r="AG7" s="92">
+      <c r="AG7" s="72">
         <v>1</v>
       </c>
-      <c r="AH7" s="93" t="s">
+      <c r="AH7" s="73" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="92">
+      <c r="C8" s="72">
         <v>50</v>
       </c>
-      <c r="D8" s="93"/>
-      <c r="S8" s="95">
+      <c r="D8" s="73"/>
+      <c r="S8" s="75">
         <v>2</v>
       </c>
-      <c r="T8" s="97">
+      <c r="T8" s="77">
         <v>81</v>
       </c>
-      <c r="U8" s="107">
+      <c r="U8" s="81">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="V8" s="97">
+      <c r="V8" s="77">
         <f>$C$7/U8</f>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="AE8" s="116" t="s">
+      <c r="AE8" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="AF8" s="112">
+      <c r="AF8" s="86">
         <v>1</v>
       </c>
-      <c r="AG8" s="85" t="s">
+      <c r="AG8" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="AH8" s="86">
+      <c r="AH8" s="66">
         <v>-1</v>
       </c>
     </row>
     <row r="9" spans="2:34" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="92">
+      <c r="C9" s="72">
         <v>1</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="D9" s="73" t="s">
         <v>57</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
-      <c r="S9" s="61" t="s">
+      <c r="S9" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="T9" s="62"/>
-      <c r="U9" s="62"/>
-      <c r="V9" s="63"/>
+      <c r="T9" s="98"/>
+      <c r="U9" s="98"/>
+      <c r="V9" s="99"/>
     </row>
     <row r="10" spans="2:34" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="92">
+      <c r="C10" s="72">
         <v>1</v>
       </c>
-      <c r="D10" s="93" t="s">
+      <c r="D10" s="73" t="s">
         <v>51</v>
       </c>
       <c r="S10" s="9">
@@ -12841,13 +12841,13 @@
       </c>
     </row>
     <row r="11" spans="2:34" ht="18" x14ac:dyDescent="0.4">
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="96">
+      <c r="C11" s="76">
         <v>50</v>
       </c>
-      <c r="D11" s="97" t="s">
+      <c r="D11" s="77" t="s">
         <v>52</v>
       </c>
       <c r="S11" s="7">
@@ -12866,14 +12866,14 @@
       </c>
     </row>
     <row r="12" spans="2:34" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="85">
+      <c r="C12" s="65">
         <f>C9*C6*V5*U5/C8</f>
         <v>0.02</v>
       </c>
-      <c r="D12" s="86"/>
+      <c r="D12" s="66"/>
       <c r="S12" s="7">
         <v>2</v>
       </c>
@@ -12906,12 +12906,12 @@
       </c>
     </row>
     <row r="14" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="S14" s="61" t="s">
+      <c r="S14" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="T14" s="62"/>
-      <c r="U14" s="62"/>
-      <c r="V14" s="63"/>
+      <c r="T14" s="98"/>
+      <c r="U14" s="98"/>
+      <c r="V14" s="99"/>
     </row>
     <row r="15" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="16"/>
@@ -12927,21 +12927,21 @@
         <v>5</v>
       </c>
       <c r="V15" s="46">
-        <f>$C$7/U15</f>
+        <f t="shared" ref="V15:V22" si="2">$C$7/U15</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="70"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="106"/>
       <c r="S16" s="47">
         <v>2</v>
       </c>
@@ -12953,27 +12953,27 @@
         <v>15</v>
       </c>
       <c r="V16" s="48">
-        <f>$C$7/U16</f>
+        <f t="shared" si="2"/>
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="17" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="65"/>
-      <c r="D17" s="66" t="s">
+      <c r="C17" s="101"/>
+      <c r="D17" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="67"/>
-      <c r="F17" s="64" t="s">
+      <c r="E17" s="103"/>
+      <c r="F17" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="65"/>
-      <c r="H17" s="64" t="s">
+      <c r="G17" s="101"/>
+      <c r="H17" s="100" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="65"/>
+      <c r="I17" s="101"/>
       <c r="S17" s="47">
         <v>2</v>
       </c>
@@ -12985,7 +12985,7 @@
         <v>13</v>
       </c>
       <c r="V17" s="48">
-        <f>$C$7/U17</f>
+        <f t="shared" si="2"/>
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
@@ -13025,7 +13025,7 @@
         <v>11</v>
       </c>
       <c r="V18" s="48">
-        <f>$C$7/U18</f>
+        <f t="shared" si="2"/>
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
@@ -13034,28 +13034,28 @@
         <v>0</v>
       </c>
       <c r="C19" s="23">
-        <f>$C$3+(EXP(B19*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" ref="C19:C30" si="3">$C$3+(EXP(B19*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
         <v>0</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
       </c>
       <c r="E19" s="23">
-        <f>$C$3+(EXP(D19*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" ref="E19:E40" si="4">$C$3+(EXP(D19*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
         <v>0</v>
       </c>
       <c r="F19" s="2">
         <v>0</v>
       </c>
       <c r="G19" s="23">
-        <f>$C$3+(EXP(F19*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" ref="G19:G60" si="5">$C$3+(EXP(F19*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
         <v>0</v>
       </c>
       <c r="H19" s="2">
         <v>0</v>
       </c>
       <c r="I19" s="3">
-        <f>$C$3+(EXP(H19*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" ref="I19:I50" si="6">$C$3+(EXP(H19*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
         <v>0</v>
       </c>
       <c r="S19" s="47">
@@ -13069,7 +13069,7 @@
         <v>30</v>
       </c>
       <c r="V19" s="48">
-        <f>$C$7/U19</f>
+        <f t="shared" si="2"/>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
@@ -13079,7 +13079,7 @@
         <v>0.05</v>
       </c>
       <c r="C20" s="23">
-        <f>$C$3+(EXP(B20*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="3"/>
         <v>2.1568233526564253E-21</v>
       </c>
       <c r="D20" s="2">
@@ -13087,7 +13087,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E20" s="23">
-        <f>$C$3+(EXP(D20*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>4.8032486005825407E-22</v>
       </c>
       <c r="F20" s="2">
@@ -13095,7 +13095,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="G20" s="23">
-        <f>$C$3+(EXP(F20*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.6746292583926853E-22</v>
       </c>
       <c r="H20" s="2">
@@ -13103,7 +13103,7 @@
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="I20" s="3">
-        <f>$C$3+(EXP(H20*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>7.0753862326635635E-23</v>
       </c>
       <c r="S20" s="42">
@@ -13117,41 +13117,41 @@
         <v>26</v>
       </c>
       <c r="V20" s="43">
-        <f>$C$7/U20</f>
+        <f t="shared" si="2"/>
         <v>3.8461538461538464E-2</v>
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B29" si="2">B20+$V$5</f>
+        <f t="shared" ref="B21:B29" si="7">B20+$V$5</f>
         <v>0.15000000000000002</v>
       </c>
       <c r="C21" s="23">
-        <f>$C$3+(EXP(B21*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="3"/>
         <v>3.485332782146486E-19</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" ref="D21:D39" si="3">D20+$V$6</f>
+        <f t="shared" ref="D21:D39" si="8">D20+$V$6</f>
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="E21" s="23">
-        <f>$C$3+(EXP(D21*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>8.0083780594918503E-21</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" ref="F21:F59" si="4">F20+$V$7</f>
+        <f t="shared" ref="F21:F59" si="9">F20+$V$7</f>
         <v>3.7500000000000006E-2</v>
       </c>
       <c r="G21" s="23">
-        <f>$C$3+(EXP(F21*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.0648279038972999E-21</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" ref="H21:H52" si="5">H20+$V$8</f>
+        <f t="shared" ref="H21:H52" si="10">H20+$V$8</f>
         <v>1.8750000000000003E-2</v>
       </c>
       <c r="I21" s="3">
-        <f>$C$3+(EXP(H21*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>2.9964854310372168E-22</v>
       </c>
       <c r="S21" s="42">
@@ -13165,41 +13165,41 @@
         <v>25</v>
       </c>
       <c r="V21" s="43">
-        <f>$C$7/U21</f>
+        <f t="shared" si="2"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="22" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.25</v>
       </c>
       <c r="C22" s="23">
-        <f>$C$3+(EXP(B22*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="3"/>
         <v>5.1755357183033894E-17</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.125</v>
       </c>
       <c r="E22" s="23">
-        <f>$C$3+(EXP(D22*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>9.9718840697446029E-20</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>6.25E-2</v>
       </c>
       <c r="G22" s="23">
-        <f>$C$3+(EXP(F22*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>4.1969394353350485E-21</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>3.125E-2</v>
       </c>
       <c r="I22" s="3">
-        <f>$C$3+(EXP(H22*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>7.2728010514325144E-22</v>
       </c>
       <c r="S22" s="49">
@@ -13213,81 +13213,81 @@
         <v>24</v>
       </c>
       <c r="V22" s="51">
-        <f>$C$7/U22</f>
+        <f t="shared" si="2"/>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="23" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.35</v>
       </c>
       <c r="C23" s="23">
-        <f>$C$3+(EXP(B23*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="3"/>
         <v>7.6812044923271107E-15</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.17499999999999999</v>
       </c>
       <c r="E23" s="23">
-        <f>$C$3+(EXP(D23*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>1.2169809979176447E-18</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="G23" s="23">
-        <f>$C$3+(EXP(F23*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.5129082861073815E-20</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>4.3749999999999997E-2</v>
       </c>
       <c r="I23" s="3">
-        <f>$C$3+(EXP(H23*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>1.5262010421940298E-21</v>
       </c>
-      <c r="S23" s="61" t="s">
+      <c r="S23" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="T23" s="62"/>
-      <c r="U23" s="62"/>
-      <c r="V23" s="63"/>
+      <c r="T23" s="98"/>
+      <c r="U23" s="98"/>
+      <c r="V23" s="99"/>
     </row>
     <row r="24" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="C24" s="23">
-        <f>$C$3+(EXP(B24*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="3"/>
         <v>1.1399918528514765E-12</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.22499999999999998</v>
       </c>
       <c r="E24" s="23">
-        <f>$C$3+(EXP(D24*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>1.4828020480775224E-17</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.11249999999999999</v>
       </c>
       <c r="G24" s="23">
-        <f>$C$3+(EXP(F24*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>5.3286012677063849E-20</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>5.6249999999999994E-2</v>
       </c>
       <c r="I24" s="3">
-        <f>$C$3+(EXP(H24*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>3.0187818531471079E-21</v>
       </c>
       <c r="S24" s="31">
@@ -13307,171 +13307,171 @@
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.54999999999999993</v>
       </c>
       <c r="C25" s="23">
-        <f>$C$3+(EXP(B25*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="3"/>
         <v>1.6918979226131959E-10</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.27499999999999997</v>
       </c>
       <c r="E25" s="23">
-        <f>$C$3+(EXP(D25*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>1.8064442677958422E-16</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.13749999999999998</v>
       </c>
       <c r="G25" s="23">
-        <f>$C$3+(EXP(F25*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.8646678393867047E-19</v>
       </c>
       <c r="H25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>6.8749999999999992E-2</v>
       </c>
       <c r="I25" s="3">
-        <f>$C$3+(EXP(H25*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>5.807289919351105E-21</v>
       </c>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.64999999999999991</v>
       </c>
       <c r="C26" s="23">
-        <f>$C$3+(EXP(B26*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="3"/>
         <v>2.5109991557439448E-8</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.32499999999999996</v>
       </c>
       <c r="E26" s="23">
-        <f>$C$3+(EXP(D26*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>2.2007017951003744E-15</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.16249999999999998</v>
       </c>
       <c r="G26" s="23">
-        <f>$C$3+(EXP(F26*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>6.5131335098095486E-19</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.1249999999999989E-2</v>
       </c>
       <c r="I26" s="3">
-        <f>$C$3+(EXP(H26*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>1.1016908841303863E-20</v>
       </c>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.74999999999999989</v>
       </c>
       <c r="C27" s="23">
-        <f>$C$3+(EXP(B27*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="3"/>
         <v>3.7266531720786451E-6</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.37499999999999994</v>
       </c>
       <c r="E27" s="23">
-        <f>$C$3+(EXP(D27*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>2.6810038484942956E-14</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.18749999999999997</v>
       </c>
       <c r="G27" s="23">
-        <f>$C$3+(EXP(F27*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>2.273787292557307E-18</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>9.3749999999999986E-2</v>
       </c>
       <c r="I27" s="3">
-        <f>$C$3+(EXP(H27*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>2.0749758332004521E-20</v>
       </c>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.84999999999999987</v>
       </c>
       <c r="C28" s="23">
-        <f>$C$3+(EXP(B28*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="3"/>
         <v>5.5308437014782972E-4</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.42499999999999993</v>
       </c>
       <c r="E28" s="23">
-        <f>$C$3+(EXP(D28*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>3.2661313408586857E-13</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.21249999999999997</v>
       </c>
       <c r="G28" s="23">
-        <f>$C$3+(EXP(F28*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>7.9367777882036805E-18</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.10624999999999998</v>
       </c>
       <c r="I28" s="3">
-        <f>$C$3+(EXP(H28*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>3.8933115047302286E-20</v>
       </c>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="7"/>
         <v>0.94999999999999984</v>
       </c>
       <c r="C29" s="23">
-        <f>$C$3+(EXP(B29*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="3"/>
         <v>8.2084998623898217E-2</v>
       </c>
       <c r="D29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.47499999999999992</v>
       </c>
       <c r="E29" s="23">
-        <f>$C$3+(EXP(D29*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>3.9789625356443517E-12</v>
       </c>
       <c r="F29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.23749999999999996</v>
       </c>
       <c r="G29" s="23">
-        <f>$C$3+(EXP(F29*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>2.7702556782856345E-17</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.11874999999999998</v>
       </c>
       <c r="I29" s="3">
-        <f>$C$3+(EXP(H29*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>7.2904097723205404E-20</v>
       </c>
     </row>
@@ -13480,31 +13480,31 @@
         <v>1</v>
       </c>
       <c r="C30" s="24">
-        <f>$C$3+(EXP(B30*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="D30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.52499999999999991</v>
       </c>
       <c r="E30" s="23">
-        <f>$C$3+(EXP(D30*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>4.8473687062509513E-11</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.26249999999999996</v>
       </c>
       <c r="G30" s="23">
-        <f>$C$3+(EXP(F30*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>9.6691904295589479E-17</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.13124999999999998</v>
       </c>
       <c r="I30" s="3">
-        <f>$C$3+(EXP(H30*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>1.3637024877746143E-19</v>
       </c>
     </row>
@@ -13512,27 +13512,27 @@
       <c r="B31" s="17"/>
       <c r="C31" s="15"/>
       <c r="D31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.57499999999999996</v>
       </c>
       <c r="E31" s="23">
-        <f>$C$3+(EXP(D31*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>5.9053039989420903E-10</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.28749999999999998</v>
       </c>
       <c r="G31" s="23">
-        <f>$C$3+(EXP(F31*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>3.374883875265451E-16</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.14374999999999999</v>
       </c>
       <c r="I31" s="3">
-        <f>$C$3+(EXP(H31*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>2.5494062891835805E-19</v>
       </c>
     </row>
@@ -13540,27 +13540,27 @@
       <c r="B32" s="17"/>
       <c r="C32" s="15"/>
       <c r="D32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.625</v>
       </c>
       <c r="E32" s="23">
-        <f>$C$3+(EXP(D32*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>7.1941330303251907E-9</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.3125</v>
       </c>
       <c r="G32" s="23">
-        <f>$C$3+(EXP(F32*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.1779506969532916E-15</v>
       </c>
       <c r="H32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.15625</v>
       </c>
       <c r="I32" s="3">
-        <f>$C$3+(EXP(H32*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>4.7645926228779048E-19</v>
       </c>
     </row>
@@ -13568,27 +13568,27 @@
       <c r="B33" s="17"/>
       <c r="C33" s="15"/>
       <c r="D33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.67500000000000004</v>
       </c>
       <c r="E33" s="23">
-        <f>$C$3+(EXP(D33*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>8.7642482194436174E-8</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.33750000000000002</v>
       </c>
       <c r="G33" s="23">
-        <f>$C$3+(EXP(F33*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>4.1114523996730492E-15</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.16875000000000001</v>
       </c>
       <c r="I33" s="3">
-        <f>$C$3+(EXP(H33*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>8.9031055357614268E-19</v>
       </c>
       <c r="S33" s="12"/>
@@ -13600,27 +13600,27 @@
       <c r="B34" s="17"/>
       <c r="C34" s="15"/>
       <c r="D34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.72500000000000009</v>
       </c>
       <c r="E34" s="23">
-        <f>$C$3+(EXP(D34*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>1.0677040100347901E-6</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.36250000000000004</v>
       </c>
       <c r="G34" s="23">
-        <f>$C$3+(EXP(F34*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.4350379408463327E-14</v>
       </c>
       <c r="H34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.18125000000000002</v>
       </c>
       <c r="I34" s="3">
-        <f>$C$3+(EXP(H34*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>1.6634865555037151E-18</v>
       </c>
       <c r="S34" s="12"/>
@@ -13632,27 +13632,27 @@
       <c r="B35" s="17"/>
       <c r="C35" s="15"/>
       <c r="D35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.77500000000000013</v>
       </c>
       <c r="E35" s="23">
-        <f>$C$3+(EXP(D35*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>1.3007297654067714E-5</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.38750000000000007</v>
       </c>
       <c r="G35" s="23">
-        <f>$C$3+(EXP(F35*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>5.0087746185560261E-14</v>
       </c>
       <c r="H35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.19375000000000003</v>
       </c>
       <c r="I35" s="3">
-        <f>$C$3+(EXP(H35*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>3.1079694954885074E-18</v>
       </c>
       <c r="S35" s="12"/>
@@ -13664,27 +13664,27 @@
       <c r="B36" s="17"/>
       <c r="C36" s="15"/>
       <c r="D36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.82500000000000018</v>
       </c>
       <c r="E36" s="23">
-        <f>$C$3+(EXP(D36*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>1.5846132511575239E-4</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.41250000000000009</v>
       </c>
       <c r="G36" s="23">
-        <f>$C$3+(EXP(F36*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.7482341263423132E-13</v>
       </c>
       <c r="H36" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.20625000000000004</v>
       </c>
       <c r="I36" s="3">
-        <f>$C$3+(EXP(H36*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>5.8066189086949072E-18</v>
       </c>
     </row>
@@ -13692,27 +13692,27 @@
       <c r="B37" s="17"/>
       <c r="C37" s="15"/>
       <c r="D37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.87500000000000022</v>
       </c>
       <c r="E37" s="23">
-        <f>$C$3+(EXP(D37*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>1.9304541362277371E-3</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.43750000000000011</v>
       </c>
       <c r="G37" s="23">
-        <f>$C$3+(EXP(F37*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>6.1019366756766178E-13</v>
       </c>
       <c r="H37" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.21875000000000006</v>
       </c>
       <c r="I37" s="3">
-        <f>$C$3+(EXP(H37*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>1.0848359765444622E-17</v>
       </c>
     </row>
@@ -13720,27 +13720,27 @@
       <c r="B38" s="17"/>
       <c r="C38" s="15"/>
       <c r="D38" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.92500000000000027</v>
       </c>
       <c r="E38" s="23">
-        <f>$C$3+(EXP(D38*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>2.3517745856009444E-2</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.46250000000000013</v>
       </c>
       <c r="G38" s="23">
-        <f>$C$3+(EXP(F38*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>2.1297851707629252E-12</v>
       </c>
       <c r="H38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.23125000000000007</v>
       </c>
       <c r="I38" s="3">
-        <f>$C$3+(EXP(H38*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>2.0267571739488127E-17</v>
       </c>
     </row>
@@ -13748,27 +13748,27 @@
       <c r="B39" s="17"/>
       <c r="C39" s="15"/>
       <c r="D39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>0.97500000000000031</v>
       </c>
       <c r="E39" s="23">
-        <f>$C$3+(EXP(D39*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>0.2865047968601942</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.48750000000000016</v>
       </c>
       <c r="G39" s="23">
-        <f>$C$3+(EXP(F39*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>7.4336806721593663E-12</v>
       </c>
       <c r="H39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.24375000000000008</v>
       </c>
       <c r="I39" s="3">
-        <f>$C$3+(EXP(H39*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>3.7864976432192083E-17</v>
       </c>
     </row>
@@ -13779,23 +13779,23 @@
         <v>1</v>
       </c>
       <c r="E40" s="24">
-        <f>$C$3+(EXP(D40*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F40" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.51250000000000018</v>
       </c>
       <c r="G40" s="23">
-        <f>$C$3+(EXP(F40*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>2.5946094982571976E-11</v>
       </c>
       <c r="H40" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.25625000000000009</v>
       </c>
       <c r="I40" s="3">
-        <f>$C$3+(EXP(H40*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>7.0741256610635084E-17</v>
       </c>
     </row>
@@ -13805,19 +13805,19 @@
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
       <c r="F41" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.5375000000000002</v>
       </c>
       <c r="G41" s="23">
-        <f>$C$3+(EXP(F41*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>9.0560769896536766E-11</v>
       </c>
       <c r="H41" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.2687500000000001</v>
       </c>
       <c r="I41" s="3">
-        <f>$C$3+(EXP(H41*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>1.3216223414942054E-16</v>
       </c>
     </row>
@@ -13827,19 +13827,19 @@
       <c r="D42" s="15"/>
       <c r="E42" s="15"/>
       <c r="F42" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.56250000000000022</v>
       </c>
       <c r="G42" s="23">
-        <f>$C$3+(EXP(F42*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>3.1608814543117973E-10</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.28125000000000011</v>
       </c>
       <c r="I42" s="3">
-        <f>$C$3+(EXP(H42*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>2.4691172713779154E-16</v>
       </c>
     </row>
@@ -13849,19 +13849,19 @@
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
       <c r="F43" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.58750000000000024</v>
       </c>
       <c r="G43" s="23">
-        <f>$C$3+(EXP(F43*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.1032560323433728E-9</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.29375000000000012</v>
       </c>
       <c r="I43" s="3">
-        <f>$C$3+(EXP(H43*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>4.6129200353071282E-16</v>
       </c>
     </row>
@@ -13871,19 +13871,19 @@
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
       <c r="F44" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.61250000000000027</v>
       </c>
       <c r="G44" s="23">
-        <f>$C$3+(EXP(F44*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>3.8507419227674793E-9</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.30625000000000013</v>
       </c>
       <c r="I44" s="3">
-        <f>$C$3+(EXP(H44*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>8.6180708825499227E-16</v>
       </c>
     </row>
@@ -13893,19 +13893,19 @@
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
       <c r="F45" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.63750000000000029</v>
       </c>
       <c r="G45" s="23">
-        <f>$C$3+(EXP(F45*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.3440409951135022E-8</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.31875000000000014</v>
       </c>
       <c r="I45" s="3">
-        <f>$C$3+(EXP(H45*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>1.6100677761817495E-15</v>
       </c>
     </row>
@@ -13915,19 +13915,19 @@
       <c r="D46" s="15"/>
       <c r="E46" s="15"/>
       <c r="F46" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.66250000000000031</v>
       </c>
       <c r="G46" s="23">
-        <f>$C$3+(EXP(F46*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>4.6911640218344654E-8</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.33125000000000016</v>
       </c>
       <c r="I46" s="3">
-        <f>$C$3+(EXP(H46*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>3.0080027815063676E-15</v>
       </c>
     </row>
@@ -13937,19 +13937,19 @@
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
       <c r="F47" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.68750000000000033</v>
       </c>
       <c r="G47" s="23">
-        <f>$C$3+(EXP(F47*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.637377130590834E-7</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.34375000000000017</v>
       </c>
       <c r="I47" s="3">
-        <f>$C$3+(EXP(H47*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>5.6196892039570783E-15</v>
       </c>
     </row>
@@ -13959,19 +13959,19 @@
       <c r="D48" s="15"/>
       <c r="E48" s="15"/>
       <c r="F48" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.71250000000000036</v>
       </c>
       <c r="G48" s="23">
-        <f>$C$3+(EXP(F48*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>5.7150077364668012E-7</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.35625000000000018</v>
       </c>
       <c r="I48" s="3">
-        <f>$C$3+(EXP(H48*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>1.049896180478124E-14</v>
       </c>
     </row>
@@ -13981,19 +13981,19 @@
       <c r="D49" s="15"/>
       <c r="E49" s="15"/>
       <c r="F49" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.73750000000000038</v>
       </c>
       <c r="G49" s="23">
-        <f>$C$3+(EXP(F49*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.9947337004816979E-6</v>
       </c>
       <c r="H49" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.36875000000000019</v>
       </c>
       <c r="I49" s="3">
-        <f>$C$3+(EXP(H49*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>1.9614643116480858E-14</v>
       </c>
     </row>
@@ -14003,19 +14003,19 @@
       <c r="D50" s="15"/>
       <c r="E50" s="15"/>
       <c r="F50" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.7625000000000004</v>
       </c>
       <c r="G50" s="23">
-        <f>$C$3+(EXP(F50*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>6.962304723488094E-6</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.3812500000000002</v>
       </c>
       <c r="I50" s="3">
-        <f>$C$3+(EXP(H50*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="6"/>
         <v>3.6644977876304056E-14</v>
       </c>
     </row>
@@ -14025,19 +14025,19 @@
       <c r="D51" s="15"/>
       <c r="E51" s="15"/>
       <c r="F51" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.78750000000000042</v>
       </c>
       <c r="G51" s="23">
-        <f>$C$3+(EXP(F51*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>2.4300831259329983E-5</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.39375000000000021</v>
       </c>
       <c r="I51" s="3">
-        <f>$C$3+(EXP(H51*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" ref="I51:I82" si="11">$C$3+(EXP(H51*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
         <v>6.8461831945061219E-14</v>
       </c>
     </row>
@@ -14047,19 +14047,19 @@
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
       <c r="F52" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.81250000000000044</v>
       </c>
       <c r="G52" s="23">
-        <f>$C$3+(EXP(F52*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>8.4818235246470971E-5</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0.40625000000000022</v>
       </c>
       <c r="I52" s="3">
-        <f>$C$3+(EXP(H52*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>1.279035409372277E-13</v>
       </c>
     </row>
@@ -14069,19 +14069,19 @@
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
       <c r="F53" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.83750000000000047</v>
       </c>
       <c r="G53" s="23">
-        <f>$C$3+(EXP(F53*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>2.9604473005686173E-4</v>
       </c>
       <c r="H53" s="2">
-        <f t="shared" ref="H53:H84" si="6">H52+$V$8</f>
+        <f t="shared" ref="H53:H84" si="12">H52+$V$8</f>
         <v>0.41875000000000023</v>
       </c>
       <c r="I53" s="3">
-        <f>$C$3+(EXP(H53*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>2.3895527346470535E-13</v>
       </c>
     </row>
@@ -14091,19 +14091,19 @@
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.86250000000000049</v>
       </c>
       <c r="G54" s="23">
-        <f>$C$3+(EXP(F54*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.0332976386476591E-3</v>
       </c>
       <c r="H54" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.43125000000000024</v>
       </c>
       <c r="I54" s="3">
-        <f>$C$3+(EXP(H54*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>4.4642722382500994E-13</v>
       </c>
     </row>
@@ -14113,19 +14113,19 @@
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
       <c r="F55" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.88750000000000051</v>
       </c>
       <c r="G55" s="23">
-        <f>$C$3+(EXP(F55*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>3.6065631360158333E-3</v>
       </c>
       <c r="H55" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.44375000000000026</v>
       </c>
       <c r="I55" s="3">
-        <f>$C$3+(EXP(H55*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>8.3403585636623067E-13</v>
       </c>
     </row>
@@ -14135,19 +14135,19 @@
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
       <c r="F56" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.91250000000000053</v>
       </c>
       <c r="G56" s="23">
-        <f>$C$3+(EXP(F56*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.2588142242434357E-2</v>
       </c>
       <c r="H56" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.45625000000000027</v>
       </c>
       <c r="I56" s="3">
-        <f>$C$3+(EXP(H56*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>1.5581841171771949E-12</v>
       </c>
     </row>
@@ -14157,19 +14157,19 @@
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
       <c r="F57" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.93750000000000056</v>
       </c>
       <c r="G57" s="23">
-        <f>$C$3+(EXP(F57*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>4.3936933623408669E-2</v>
       </c>
       <c r="H57" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.46875000000000028</v>
       </c>
       <c r="I57" s="3">
-        <f>$C$3+(EXP(H57*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>2.9110711780188537E-12</v>
       </c>
     </row>
@@ -14179,19 +14179,19 @@
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
       <c r="F58" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.96250000000000058</v>
       </c>
       <c r="G58" s="23">
-        <f>$C$3+(EXP(F58*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>0.15335496684493283</v>
       </c>
       <c r="H58" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.48125000000000029</v>
       </c>
       <c r="I58" s="3">
-        <f>$C$3+(EXP(H58*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>5.4385969602986439E-12</v>
       </c>
     </row>
@@ -14201,19 +14201,19 @@
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
       <c r="F59" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>0.9875000000000006</v>
       </c>
       <c r="G59" s="23">
-        <f>$C$3+(EXP(F59*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>0.53526142851900549</v>
       </c>
       <c r="H59" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.4937500000000003</v>
       </c>
       <c r="I59" s="3">
-        <f>$C$3+(EXP(H59*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>1.0160636785348578E-11</v>
       </c>
     </row>
@@ -14227,15 +14227,15 @@
         <v>1.0000000000000007</v>
       </c>
       <c r="G60" s="26">
-        <f>$C$3+(EXP(F60*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000355</v>
       </c>
       <c r="H60" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.50625000000000031</v>
       </c>
       <c r="I60" s="3">
-        <f>$C$3+(EXP(H60*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>1.8982568599332073E-11</v>
       </c>
     </row>
@@ -14247,11 +14247,11 @@
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
       <c r="H61" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.51875000000000027</v>
       </c>
       <c r="I61" s="3">
-        <f>$C$3+(EXP(H61*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>3.5464107047549455E-11</v>
       </c>
     </row>
@@ -14263,11 +14263,11 @@
       <c r="F62" s="15"/>
       <c r="G62" s="15"/>
       <c r="H62" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.53125000000000022</v>
       </c>
       <c r="I62" s="3">
-        <f>$C$3+(EXP(H62*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>6.6255674625695089E-11</v>
       </c>
     </row>
@@ -14279,11 +14279,11 @@
       <c r="F63" s="15"/>
       <c r="G63" s="15"/>
       <c r="H63" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.54375000000000018</v>
       </c>
       <c r="I63" s="3">
-        <f>$C$3+(EXP(H63*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>1.2378189627656654E-10</v>
       </c>
     </row>
@@ -14295,11 +14295,11 @@
       <c r="F64" s="15"/>
       <c r="G64" s="15"/>
       <c r="H64" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.55625000000000013</v>
       </c>
       <c r="I64" s="3">
-        <f>$C$3+(EXP(H64*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>2.3125502732215755E-10</v>
       </c>
     </row>
@@ -14311,11 +14311,11 @@
       <c r="F65" s="15"/>
       <c r="G65" s="15"/>
       <c r="H65" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.56875000000000009</v>
       </c>
       <c r="I65" s="3">
-        <f>$C$3+(EXP(H65*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>4.320412699306649E-10</v>
       </c>
     </row>
@@ -14327,11 +14327,11 @@
       <c r="F66" s="15"/>
       <c r="G66" s="15"/>
       <c r="H66" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.58125000000000004</v>
       </c>
       <c r="I66" s="3">
-        <f>$C$3+(EXP(H66*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>8.0715935599201584E-10</v>
       </c>
     </row>
@@ -14343,11 +14343,11 @@
       <c r="F67" s="15"/>
       <c r="G67" s="15"/>
       <c r="H67" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.59375</v>
       </c>
       <c r="I67" s="3">
-        <f>$C$3+(EXP(H67*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>1.5079722038358418E-9</v>
       </c>
     </row>
@@ -14359,11 +14359,11 @@
       <c r="F68" s="15"/>
       <c r="G68" s="15"/>
       <c r="H68" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.60624999999999996</v>
       </c>
       <c r="I68" s="3">
-        <f>$C$3+(EXP(H68*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>2.817262973736628E-9</v>
       </c>
     </row>
@@ -14375,11 +14375,11 @@
       <c r="F69" s="15"/>
       <c r="G69" s="15"/>
       <c r="H69" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.61874999999999991</v>
       </c>
       <c r="I69" s="3">
-        <f>$C$3+(EXP(H69*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>5.2633401617071044E-9</v>
       </c>
     </row>
@@ -14391,11 +14391,11 @@
       <c r="F70" s="15"/>
       <c r="G70" s="15"/>
       <c r="H70" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.63124999999999987</v>
       </c>
       <c r="I70" s="3">
-        <f>$C$3+(EXP(H70*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>9.8332139797000909E-9</v>
       </c>
     </row>
@@ -14407,11 +14407,11 @@
       <c r="F71" s="15"/>
       <c r="G71" s="15"/>
       <c r="H71" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.64374999999999982</v>
       </c>
       <c r="I71" s="3">
-        <f>$C$3+(EXP(H71*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>1.8370862266140877E-8</v>
       </c>
     </row>
@@ -14423,11 +14423,11 @@
       <c r="F72" s="15"/>
       <c r="G72" s="15"/>
       <c r="H72" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.65624999999999978</v>
       </c>
       <c r="I72" s="3">
-        <f>$C$3+(EXP(H72*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>3.4321289163261772E-8</v>
       </c>
     </row>
@@ -14439,11 +14439,11 @@
       <c r="F73" s="15"/>
       <c r="G73" s="15"/>
       <c r="H73" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.66874999999999973</v>
       </c>
       <c r="I73" s="3">
-        <f>$C$3+(EXP(H73*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>6.4120609733126306E-8</v>
       </c>
     </row>
@@ -14455,11 +14455,11 @@
       <c r="F74" s="15"/>
       <c r="G74" s="15"/>
       <c r="H74" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.68124999999999969</v>
       </c>
       <c r="I74" s="3">
-        <f>$C$3+(EXP(H74*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>1.1979306992200262E-7</v>
       </c>
     </row>
@@ -14471,11 +14471,11 @@
       <c r="F75" s="15"/>
       <c r="G75" s="15"/>
       <c r="H75" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.69374999999999964</v>
       </c>
       <c r="I75" s="3">
-        <f>$C$3+(EXP(H75*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>2.238029186101771E-7</v>
       </c>
     </row>
@@ -14487,11 +14487,11 @@
       <c r="F76" s="15"/>
       <c r="G76" s="15"/>
       <c r="H76" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.7062499999999996</v>
       </c>
       <c r="I76" s="3">
-        <f>$C$3+(EXP(H76*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>4.1811889795499329E-7</v>
       </c>
     </row>
@@ -14503,11 +14503,11 @@
       <c r="F77" s="15"/>
       <c r="G77" s="15"/>
       <c r="H77" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.71874999999999956</v>
       </c>
       <c r="I77" s="3">
-        <f>$C$3+(EXP(H77*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>7.8114894083043226E-7</v>
       </c>
     </row>
@@ -14519,11 +14519,11 @@
       <c r="F78" s="15"/>
       <c r="G78" s="15"/>
       <c r="H78" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.73124999999999951</v>
       </c>
       <c r="I78" s="3">
-        <f>$C$3+(EXP(H78*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>1.4593783508589176E-6</v>
       </c>
     </row>
@@ -14535,11 +14535,11 @@
       <c r="F79" s="15"/>
       <c r="G79" s="15"/>
       <c r="H79" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.74374999999999947</v>
       </c>
       <c r="I79" s="3">
-        <f>$C$3+(EXP(H79*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>2.7264777043562575E-6</v>
       </c>
     </row>
@@ -14551,11 +14551,11 @@
       <c r="F80" s="15"/>
       <c r="G80" s="15"/>
       <c r="H80" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.75624999999999942</v>
       </c>
       <c r="I80" s="3">
-        <f>$C$3+(EXP(H80*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>5.093730949192664E-6</v>
       </c>
     </row>
@@ -14567,11 +14567,11 @@
       <c r="F81" s="15"/>
       <c r="G81" s="15"/>
       <c r="H81" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.76874999999999938</v>
       </c>
       <c r="I81" s="3">
-        <f>$C$3+(EXP(H81*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>9.5163422540765913E-6</v>
       </c>
     </row>
@@ -14583,11 +14583,11 @@
       <c r="F82" s="15"/>
       <c r="G82" s="15"/>
       <c r="H82" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.78124999999999933</v>
       </c>
       <c r="I82" s="3">
-        <f>$C$3+(EXP(H82*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="11"/>
         <v>1.7778867945719909E-5</v>
       </c>
     </row>
@@ -14599,11 +14599,11 @@
       <c r="F83" s="15"/>
       <c r="G83" s="15"/>
       <c r="H83" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.79374999999999929</v>
       </c>
       <c r="I83" s="3">
-        <f>$C$3+(EXP(H83*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" ref="I83:I100" si="13">$C$3+(EXP(H83*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
         <v>3.3215298167312543E-5</v>
       </c>
     </row>
@@ -14615,11 +14615,11 @@
       <c r="F84" s="15"/>
       <c r="G84" s="15"/>
       <c r="H84" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.80624999999999925</v>
       </c>
       <c r="I84" s="3">
-        <f>$C$3+(EXP(H84*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>6.2054346525987564E-5</v>
       </c>
     </row>
@@ -14631,11 +14631,11 @@
       <c r="F85" s="15"/>
       <c r="G85" s="15"/>
       <c r="H85" s="2">
-        <f t="shared" ref="H85:H99" si="7">H84+$V$8</f>
+        <f t="shared" ref="H85:H99" si="14">H84+$V$8</f>
         <v>0.8187499999999992</v>
       </c>
       <c r="I85" s="3">
-        <f>$C$3+(EXP(H85*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>1.1593278203827371E-4</v>
       </c>
     </row>
@@ -14647,11 +14647,11 @@
       <c r="F86" s="15"/>
       <c r="G86" s="15"/>
       <c r="H86" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.83124999999999916</v>
       </c>
       <c r="I86" s="3">
-        <f>$C$3+(EXP(H86*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>2.1659095137687581E-4</v>
       </c>
     </row>
@@ -14663,11 +14663,11 @@
       <c r="F87" s="15"/>
       <c r="G87" s="15"/>
       <c r="H87" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.84374999999999911</v>
       </c>
       <c r="I87" s="3">
-        <f>$C$3+(EXP(H87*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>4.0464516932624728E-4</v>
       </c>
     </row>
@@ -14679,11 +14679,11 @@
       <c r="F88" s="15"/>
       <c r="G88" s="15"/>
       <c r="H88" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.85624999999999907</v>
       </c>
       <c r="I88" s="3">
-        <f>$C$3+(EXP(H88*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>7.5597670178823332E-4</v>
       </c>
     </row>
@@ -14695,11 +14695,11 @@
       <c r="F89" s="15"/>
       <c r="G89" s="15"/>
       <c r="H89" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.86874999999999902</v>
       </c>
       <c r="I89" s="3">
-        <f>$C$3+(EXP(H89*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>1.4123504170288116E-3</v>
       </c>
     </row>
@@ -14711,11 +14711,11 @@
       <c r="F90" s="15"/>
       <c r="G90" s="15"/>
       <c r="H90" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.88124999999999898</v>
       </c>
       <c r="I90" s="3">
-        <f>$C$3+(EXP(H90*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>2.6386179570917906E-3</v>
       </c>
     </row>
@@ -14727,11 +14727,11 @@
       <c r="F91" s="15"/>
       <c r="G91" s="15"/>
       <c r="H91" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.89374999999999893</v>
       </c>
       <c r="I91" s="3">
-        <f>$C$3+(EXP(H91*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>4.9295873315447717E-3</v>
       </c>
     </row>
@@ -14743,11 +14743,11 @@
       <c r="F92" s="15"/>
       <c r="G92" s="15"/>
       <c r="H92" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.90624999999999889</v>
       </c>
       <c r="I92" s="3">
-        <f>$C$3+(EXP(H92*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>9.2096816039676163E-3</v>
       </c>
     </row>
@@ -14759,11 +14759,11 @@
       <c r="F93" s="15"/>
       <c r="G93" s="15"/>
       <c r="H93" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.91874999999999885</v>
       </c>
       <c r="I93" s="3">
-        <f>$C$3+(EXP(H93*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>1.7205950425850405E-2</v>
       </c>
     </row>
@@ -14775,11 +14775,11 @@
       <c r="F94" s="15"/>
       <c r="G94" s="15"/>
       <c r="H94" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.9312499999999988</v>
       </c>
       <c r="I94" s="3">
-        <f>$C$3+(EXP(H94*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>3.214494732687425E-2</v>
       </c>
     </row>
@@ -14791,11 +14791,11 @@
       <c r="F95" s="15"/>
       <c r="G95" s="15"/>
       <c r="H95" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.94374999999999876</v>
       </c>
       <c r="I95" s="3">
-        <f>$C$3+(EXP(H95*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>6.0054667895304108E-2</v>
       </c>
     </row>
@@ -14807,11 +14807,11 @@
       <c r="F96" s="15"/>
       <c r="G96" s="15"/>
       <c r="H96" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.95624999999999871</v>
       </c>
       <c r="I96" s="3">
-        <f>$C$3+(EXP(H96*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>0.11219689052033657</v>
       </c>
     </row>
@@ -14823,11 +14823,11 @@
       <c r="F97" s="15"/>
       <c r="G97" s="15"/>
       <c r="H97" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.96874999999999867</v>
       </c>
       <c r="I97" s="3">
-        <f>$C$3+(EXP(H97*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>0.20961138715108443</v>
       </c>
     </row>
@@ -14839,11 +14839,11 @@
       <c r="F98" s="15"/>
       <c r="G98" s="15"/>
       <c r="H98" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.98124999999999862</v>
       </c>
       <c r="I98" s="3">
-        <f>$C$3+(EXP(H98*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>0.39160562667677118</v>
       </c>
     </row>
@@ -14855,11 +14855,11 @@
       <c r="F99" s="15"/>
       <c r="G99" s="15"/>
       <c r="H99" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.99374999999999858</v>
       </c>
       <c r="I99" s="3">
-        <f>$C$3+(EXP(H99*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>0.73161562894658982</v>
       </c>
     </row>
@@ -14875,7 +14875,7 @@
         <v>0.99999999999999856</v>
       </c>
       <c r="I100" s="5">
-        <f>$C$3+(EXP(H100*$C$8/$C$7)-1)/(EXP($C$8)-1)*($C$4-$C$3)</f>
+        <f t="shared" si="13"/>
         <v>0.99999999999992906</v>
       </c>
     </row>
@@ -14904,8 +14904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AC105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14917,140 +14917,140 @@
   <sheetData>
     <row r="1" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="80"/>
-      <c r="F2" s="98" t="s">
+      <c r="C2" s="108"/>
+      <c r="D2" s="109"/>
+      <c r="F2" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="99"/>
-      <c r="H2" s="99"/>
-      <c r="I2" s="100"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="115"/>
       <c r="J2" s="58"/>
-      <c r="V2" s="78" t="s">
+      <c r="V2" s="107" t="s">
         <v>34</v>
       </c>
-      <c r="W2" s="79"/>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="79"/>
-      <c r="Z2" s="80"/>
+      <c r="W2" s="108"/>
+      <c r="X2" s="108"/>
+      <c r="Y2" s="108"/>
+      <c r="Z2" s="109"/>
     </row>
     <row r="3" spans="2:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="82">
+      <c r="C3" s="62">
         <v>5</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="101" t="s">
+      <c r="F3" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="102"/>
-      <c r="H3" s="102"/>
-      <c r="I3" s="103"/>
+      <c r="G3" s="111"/>
+      <c r="H3" s="111"/>
+      <c r="I3" s="112"/>
       <c r="J3" s="59"/>
-      <c r="V3" s="113" t="s">
+      <c r="V3" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="W3" s="109" t="s">
+      <c r="W3" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="X3" s="109" t="s">
+      <c r="X3" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="Y3" s="108" t="s">
+      <c r="Y3" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="Z3" s="105" t="s">
+      <c r="Z3" s="79" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="92">
+      <c r="C4" s="72">
         <v>0.01</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="D4" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="104" t="s">
+      <c r="F4" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="105" t="s">
+      <c r="G4" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="104" t="s">
+      <c r="H4" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="105" t="s">
+      <c r="I4" s="79" t="s">
         <v>9</v>
       </c>
       <c r="J4" s="60"/>
-      <c r="V4" s="101" t="s">
+      <c r="V4" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="W4" s="102"/>
-      <c r="X4" s="102"/>
-      <c r="Y4" s="102"/>
-      <c r="Z4" s="103"/>
+      <c r="W4" s="111"/>
+      <c r="X4" s="111"/>
+      <c r="Y4" s="111"/>
+      <c r="Z4" s="112"/>
     </row>
     <row r="5" spans="2:26" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="74" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="92">
+      <c r="C5" s="72">
         <f>C4/2</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D5" s="93" t="s">
+      <c r="D5" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="119">
+      <c r="F5" s="93">
         <v>2</v>
       </c>
-      <c r="G5" s="120">
+      <c r="G5" s="94">
         <v>6</v>
       </c>
-      <c r="H5" s="121">
+      <c r="H5" s="95">
         <f>G5-F5+1</f>
         <v>5</v>
       </c>
-      <c r="I5" s="122">
+      <c r="I5" s="96">
         <f>$C$3/H5</f>
         <v>1</v>
       </c>
       <c r="J5" s="16"/>
-      <c r="V5" s="114" t="s">
+      <c r="V5" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="W5" s="110">
+      <c r="W5" s="84">
         <v>0</v>
       </c>
-      <c r="X5" s="110" t="s">
+      <c r="X5" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="Y5" s="90">
+      <c r="Y5" s="70">
         <v>1</v>
       </c>
-      <c r="Z5" s="106" t="s">
+      <c r="Z5" s="80" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:26" ht="18" x14ac:dyDescent="0.4">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="92">
+      <c r="C6" s="72">
         <v>0.01</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="D6" s="73" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="9">
@@ -15068,31 +15068,31 @@
         <v>0.5</v>
       </c>
       <c r="J6" s="16"/>
-      <c r="V6" s="115" t="s">
+      <c r="V6" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="W6" s="111">
+      <c r="W6" s="85">
         <v>0</v>
       </c>
-      <c r="X6" s="111" t="s">
+      <c r="X6" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="Y6" s="92">
+      <c r="Y6" s="72">
         <v>0</v>
       </c>
-      <c r="Z6" s="93" t="s">
+      <c r="Z6" s="73" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:26" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="85">
+      <c r="C7" s="65">
         <f>C6/2</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="66" t="s">
         <v>50</v>
       </c>
       <c r="F7" s="7">
@@ -15110,30 +15110,30 @@
         <v>0.25</v>
       </c>
       <c r="J7" s="16"/>
-      <c r="V7" s="115" t="s">
+      <c r="V7" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="W7" s="111">
+      <c r="W7" s="85">
         <v>1</v>
       </c>
-      <c r="X7" s="111" t="s">
+      <c r="X7" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="Y7" s="92">
+      <c r="Y7" s="72">
         <v>1</v>
       </c>
-      <c r="Z7" s="93" t="s">
+      <c r="Z7" s="73" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:26" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B8" s="89" t="s">
+      <c r="B8" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="90">
+      <c r="C8" s="70">
         <v>1000</v>
       </c>
-      <c r="D8" s="106" t="s">
+      <c r="D8" s="80" t="s">
         <v>57</v>
       </c>
       <c r="F8" s="33">
@@ -15151,30 +15151,30 @@
         <v>0.125</v>
       </c>
       <c r="J8" s="16"/>
-      <c r="V8" s="115" t="s">
+      <c r="V8" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="W8" s="111">
+      <c r="W8" s="85">
         <v>273.14999999999998</v>
       </c>
-      <c r="X8" s="111" t="s">
+      <c r="X8" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="Y8" s="92">
+      <c r="Y8" s="72">
         <v>0</v>
       </c>
-      <c r="Z8" s="93" t="s">
+      <c r="Z8" s="73" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:26" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="92">
+      <c r="C9" s="72">
         <v>0.59</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="D9" s="73" t="s">
         <v>51</v>
       </c>
       <c r="F9" s="29">
@@ -15192,83 +15192,83 @@
         <v>6.25E-2</v>
       </c>
       <c r="J9" s="12"/>
-      <c r="V9" s="116" t="s">
+      <c r="V9" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="W9" s="112">
+      <c r="W9" s="86">
         <v>1</v>
       </c>
-      <c r="X9" s="112" t="s">
+      <c r="X9" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="Y9" s="85" t="s">
+      <c r="Y9" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="Z9" s="86">
+      <c r="Z9" s="66">
         <v>-1</v>
       </c>
     </row>
     <row r="10" spans="2:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="94" t="s">
+      <c r="B10" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="92">
+      <c r="C10" s="72">
         <v>4189</v>
       </c>
-      <c r="D10" s="93" t="s">
+      <c r="D10" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="V10" s="101" t="s">
+      <c r="V10" s="110" t="s">
         <v>70</v>
       </c>
-      <c r="W10" s="102"/>
-      <c r="X10" s="102"/>
-      <c r="Y10" s="102"/>
-      <c r="Z10" s="103"/>
+      <c r="W10" s="111"/>
+      <c r="X10" s="111"/>
+      <c r="Y10" s="111"/>
+      <c r="Z10" s="112"/>
     </row>
     <row r="11" spans="2:26" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="92">
+      <c r="C11" s="72">
         <v>273.14999999999998</v>
       </c>
-      <c r="D11" s="93" t="s">
+      <c r="D11" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="68" t="s">
+      <c r="F11" s="104" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="70"/>
-      <c r="V11" s="114" t="s">
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="106"/>
+      <c r="V11" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="W11" s="110">
+      <c r="W11" s="84">
         <v>0</v>
       </c>
-      <c r="X11" s="111" t="s">
+      <c r="X11" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="Y11" s="90">
+      <c r="Y11" s="70">
         <v>0</v>
       </c>
-      <c r="Z11" s="106" t="s">
+      <c r="Z11" s="80" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="2:26" ht="18" x14ac:dyDescent="0.4">
-      <c r="B12" s="94" t="s">
+      <c r="B12" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="92">
+      <c r="C12" s="72">
         <f>1.5</f>
         <v>1.5</v>
       </c>
-      <c r="D12" s="93" t="s">
+      <c r="D12" s="73" t="s">
         <v>49</v>
       </c>
       <c r="G12" t="s">
@@ -15283,159 +15283,159 @@
       <c r="K12" t="s">
         <v>40</v>
       </c>
-      <c r="V12" s="115" t="s">
+      <c r="V12" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="W12" s="111">
+      <c r="W12" s="85">
         <v>1</v>
       </c>
-      <c r="X12" s="111" t="s">
+      <c r="X12" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="Y12" s="92">
+      <c r="Y12" s="72">
         <v>0</v>
       </c>
-      <c r="Z12" s="93" t="s">
+      <c r="Z12" s="73" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="13" spans="2:26" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="92">
+      <c r="C13" s="72">
         <v>10000</v>
       </c>
-      <c r="D13" s="93" t="s">
+      <c r="D13" s="73" t="s">
         <v>68</v>
       </c>
       <c r="F13" t="s">
         <v>35</v>
       </c>
-      <c r="V13" s="115" t="s">
+      <c r="V13" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="W13" s="111">
+      <c r="W13" s="85">
         <v>1</v>
       </c>
-      <c r="X13" s="111" t="s">
+      <c r="X13" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="Y13" s="92">
+      <c r="Y13" s="72">
         <v>1</v>
       </c>
-      <c r="Z13" s="93" t="s">
+      <c r="Z13" s="73" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:26" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="95" t="s">
+      <c r="B14" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="96">
+      <c r="C14" s="76">
         <v>373.15</v>
       </c>
-      <c r="D14" s="97" t="s">
+      <c r="D14" s="77" t="s">
         <v>66</v>
       </c>
       <c r="F14" t="s">
         <v>36</v>
       </c>
-      <c r="V14" s="115" t="s">
+      <c r="V14" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="W14" s="111">
+      <c r="W14" s="85">
         <v>0</v>
       </c>
-      <c r="X14" s="111" t="s">
+      <c r="X14" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="Y14" s="92">
+      <c r="Y14" s="72">
         <v>273.14999999999998</v>
       </c>
-      <c r="Z14" s="93" t="s">
+      <c r="Z14" s="73" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" spans="2:26" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="117">
+      <c r="C15" s="91">
         <f>C4*2+C6*2</f>
         <v>0.04</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="V15" s="116" t="s">
+      <c r="V15" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="W15" s="112" t="s">
+      <c r="W15" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="X15" s="112">
+      <c r="X15" s="86">
         <v>-1</v>
       </c>
-      <c r="Y15" s="85">
+      <c r="Y15" s="65">
         <v>1</v>
       </c>
-      <c r="Z15" s="86" t="s">
+      <c r="Z15" s="66" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="2:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="84" t="s">
+      <c r="B16" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="118">
+      <c r="C16" s="92">
         <f>C8*C12*C4*C6</f>
         <v>0.15</v>
       </c>
-      <c r="D16" s="86" t="s">
+      <c r="D16" s="66" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="104" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="70"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="105"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="105"/>
+      <c r="G20" s="105"/>
+      <c r="H20" s="105"/>
+      <c r="I20" s="105"/>
+      <c r="J20" s="105"/>
+      <c r="K20" s="106"/>
     </row>
     <row r="21" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="75" t="s">
+      <c r="B21" s="116" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="75" t="s">
+      <c r="C21" s="117"/>
+      <c r="D21" s="118"/>
+      <c r="E21" s="116" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="76"/>
-      <c r="G21" s="75" t="s">
+      <c r="F21" s="118"/>
+      <c r="G21" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="76"/>
-      <c r="I21" s="72" t="s">
+      <c r="H21" s="118"/>
+      <c r="I21" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="J21" s="73"/>
-      <c r="K21" s="74"/>
+      <c r="J21" s="121"/>
+      <c r="K21" s="122"/>
     </row>
     <row r="22" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="71"/>
+      <c r="C22" s="119"/>
       <c r="D22" s="28" t="s">
         <v>29</v>
       </c>
@@ -15468,21 +15468,21 @@
         <v>0</v>
       </c>
       <c r="D23" s="1">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*B23/$C$16/$C$10)</f>
+        <f t="shared" ref="D23:D29" si="1">$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*B23/$C$16/$C$10)</f>
         <v>273.14999999999998</v>
       </c>
       <c r="E23" s="36">
         <v>0</v>
       </c>
       <c r="F23" s="1">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E23/$C$16/$C$10)</f>
+        <f t="shared" ref="F23:F34" si="2">$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E23/$C$16/$C$10)</f>
         <v>273.14999999999998</v>
       </c>
       <c r="G23" s="36">
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G23/$C$16/$C$10)</f>
+        <f t="shared" ref="H23:H44" si="3">$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G23/$C$16/$C$10)</f>
         <v>273.14999999999998</v>
       </c>
       <c r="I23" s="36">
@@ -15493,7 +15493,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="1">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I23/$C$16/$C$10)</f>
+        <f t="shared" ref="K23:K64" si="4">$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I23/$C$16/$C$10)</f>
         <v>273.14999999999998</v>
       </c>
     </row>
@@ -15503,11 +15503,11 @@
         <v>0.5</v>
       </c>
       <c r="C24" s="44">
-        <f t="shared" ref="C24:C29" si="1">B24*-1</f>
+        <f t="shared" ref="C24:C29" si="5">B24*-1</f>
         <v>-0.5</v>
       </c>
       <c r="D24" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*B24/$C$16/$C$10)</f>
+        <f t="shared" si="1"/>
         <v>300.41110549618935</v>
       </c>
       <c r="E24" s="7">
@@ -15515,7 +15515,7 @@
         <v>0.25</v>
       </c>
       <c r="F24" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E24/$C$16/$C$10)</f>
+        <f t="shared" si="2"/>
         <v>287.86289985946837</v>
       </c>
       <c r="G24" s="7">
@@ -15523,7 +15523,7 @@
         <v>0.125</v>
       </c>
       <c r="H24" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G24/$C$16/$C$10)</f>
+        <f t="shared" si="3"/>
         <v>280.79898476977547</v>
       </c>
       <c r="I24" s="7">
@@ -15535,7 +15535,7 @@
         <v>4.9375</v>
       </c>
       <c r="K24" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I24/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>277.05056439800256</v>
       </c>
       <c r="V24">
@@ -15566,11 +15566,11 @@
         <v>1.5</v>
       </c>
       <c r="C25" s="44">
+        <f t="shared" si="5"/>
+        <v>-1.5</v>
+      </c>
+      <c r="D25" s="3">
         <f t="shared" si="1"/>
-        <v>-1.5</v>
-      </c>
-      <c r="D25" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*B25/$C$16/$C$10)</f>
         <v>334.66423808071772</v>
       </c>
       <c r="E25" s="7">
@@ -15578,7 +15578,7 @@
         <v>0.75</v>
       </c>
       <c r="F25" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E25/$C$16/$C$10)</f>
+        <f t="shared" si="2"/>
         <v>311.11310620341936</v>
       </c>
       <c r="G25" s="7">
@@ -15586,7 +15586,7 @@
         <v>0.375</v>
       </c>
       <c r="H25" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G25/$C$16/$C$10)</f>
+        <f t="shared" si="3"/>
         <v>294.3864971598008</v>
       </c>
       <c r="I25" s="7">
@@ -15598,7 +15598,7 @@
         <v>4.8125</v>
       </c>
       <c r="K25" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I25/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>284.40119559103954</v>
       </c>
       <c r="V25">
@@ -15625,31 +15625,31 @@
     </row>
     <row r="26" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B26" s="7">
-        <f t="shared" ref="B26:B28" si="2">(B25+$I$5)</f>
+        <f t="shared" ref="B26:B28" si="6">(B25+$I$5)</f>
         <v>2.5</v>
       </c>
       <c r="C26" s="44">
+        <f t="shared" si="5"/>
+        <v>-2.5</v>
+      </c>
+      <c r="D26" s="3">
         <f t="shared" si="1"/>
-        <v>-2.5</v>
-      </c>
-      <c r="D26" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*B26/$C$16/$C$10)</f>
         <v>352.78738821422314</v>
       </c>
       <c r="E26" s="7">
-        <f t="shared" ref="E26:E33" si="3">E25+$I$6</f>
+        <f t="shared" ref="E26:E33" si="7">E25+$I$6</f>
         <v>1.25</v>
       </c>
       <c r="F26" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E26/$C$16/$C$10)</f>
+        <f t="shared" si="2"/>
         <v>328.02504926786412</v>
       </c>
       <c r="G26" s="7">
-        <f t="shared" ref="G26:G43" si="4">G25+$I$7</f>
+        <f t="shared" ref="G26:G43" si="8">G25+$I$7</f>
         <v>0.625</v>
       </c>
       <c r="H26" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G26/$C$16/$C$10)</f>
+        <f t="shared" si="3"/>
         <v>305.97489245848885</v>
       </c>
       <c r="I26" s="7">
@@ -15657,11 +15657,11 @@
         <v>0.3125</v>
       </c>
       <c r="J26" s="55">
-        <f t="shared" ref="J26:J63" si="5">J25-$I$8</f>
+        <f t="shared" ref="J26:J63" si="9">J25-$I$8</f>
         <v>4.6875</v>
       </c>
       <c r="K26" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I26/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>291.18957812363874</v>
       </c>
       <c r="V26">
@@ -15688,43 +15688,43 @@
     </row>
     <row r="27" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B27" s="7">
+        <f t="shared" si="6"/>
+        <v>3.5</v>
+      </c>
+      <c r="C27" s="44">
+        <f t="shared" si="5"/>
+        <v>-3.5</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="1"/>
+        <v>362.37625048692314</v>
+      </c>
+      <c r="E27" s="7">
+        <f t="shared" si="7"/>
+        <v>1.75</v>
+      </c>
+      <c r="F27" s="3">
         <f t="shared" si="2"/>
-        <v>3.5</v>
-      </c>
-      <c r="C27" s="44">
-        <f t="shared" si="1"/>
-        <v>-3.5</v>
-      </c>
-      <c r="D27" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*B27/$C$16/$C$10)</f>
-        <v>362.37625048692314</v>
-      </c>
-      <c r="E27" s="7">
+        <v>340.32660969205517</v>
+      </c>
+      <c r="G27" s="7">
+        <f t="shared" si="8"/>
+        <v>0.875</v>
+      </c>
+      <c r="H27" s="3">
         <f t="shared" si="3"/>
-        <v>1.75</v>
-      </c>
-      <c r="F27" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E27/$C$16/$C$10)</f>
-        <v>340.32660969205517</v>
-      </c>
-      <c r="G27" s="7">
+        <v>315.85829876156163</v>
+      </c>
+      <c r="I27" s="7">
+        <f t="shared" ref="I27:I44" si="10">I26+$I$8</f>
+        <v>0.4375</v>
+      </c>
+      <c r="J27" s="55">
+        <f t="shared" si="9"/>
+        <v>4.5625</v>
+      </c>
+      <c r="K27" s="3">
         <f t="shared" si="4"/>
-        <v>0.875</v>
-      </c>
-      <c r="H27" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G27/$C$16/$C$10)</f>
-        <v>315.85829876156163</v>
-      </c>
-      <c r="I27" s="7">
-        <f t="shared" ref="I27:I44" si="6">I26+$I$8</f>
-        <v>0.4375</v>
-      </c>
-      <c r="J27" s="55">
-        <f t="shared" si="5"/>
-        <v>4.5625</v>
-      </c>
-      <c r="K27" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I27/$C$16/$C$10)</f>
         <v>297.45871831020537</v>
       </c>
       <c r="V27">
@@ -15751,43 +15751,43 @@
     </row>
     <row r="28" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B28" s="7">
+        <f t="shared" si="6"/>
+        <v>4.5</v>
+      </c>
+      <c r="C28" s="44">
+        <f t="shared" si="5"/>
+        <v>-4.5</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="1"/>
+        <v>367.44966647738181</v>
+      </c>
+      <c r="E28" s="7">
+        <f t="shared" si="7"/>
+        <v>2.25</v>
+      </c>
+      <c r="F28" s="3">
         <f t="shared" si="2"/>
-        <v>4.5</v>
-      </c>
-      <c r="C28" s="44">
-        <f t="shared" si="1"/>
-        <v>-4.5</v>
-      </c>
-      <c r="D28" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*B28/$C$16/$C$10)</f>
-        <v>367.44966647738181</v>
-      </c>
-      <c r="E28" s="7">
+        <v>349.27462875133</v>
+      </c>
+      <c r="G28" s="7">
+        <f t="shared" si="8"/>
+        <v>1.125</v>
+      </c>
+      <c r="H28" s="3">
         <f t="shared" si="3"/>
-        <v>2.25</v>
-      </c>
-      <c r="F28" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E28/$C$16/$C$10)</f>
-        <v>349.27462875133</v>
-      </c>
-      <c r="G28" s="7">
+        <v>324.28756939255885</v>
+      </c>
+      <c r="I28" s="7">
+        <f t="shared" si="10"/>
+        <v>0.5625</v>
+      </c>
+      <c r="J28" s="55">
+        <f t="shared" si="9"/>
+        <v>4.4375</v>
+      </c>
+      <c r="K28" s="3">
         <f t="shared" si="4"/>
-        <v>1.125</v>
-      </c>
-      <c r="H28" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G28/$C$16/$C$10)</f>
-        <v>324.28756939255885</v>
-      </c>
-      <c r="I28" s="7">
-        <f t="shared" si="6"/>
-        <v>0.5625</v>
-      </c>
-      <c r="J28" s="55">
-        <f t="shared" si="5"/>
-        <v>4.4375</v>
-      </c>
-      <c r="K28" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I28/$C$16/$C$10)</f>
         <v>303.24833291870561</v>
       </c>
       <c r="V28">
@@ -15814,43 +15814,43 @@
     </row>
     <row r="29" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="7">
-        <f t="shared" ref="B29" si="7">(B28+$I$5/2)</f>
+        <f t="shared" ref="B29" si="11">(B28+$I$5/2)</f>
         <v>5</v>
       </c>
       <c r="C29" s="44">
+        <f t="shared" si="5"/>
+        <v>-5</v>
+      </c>
+      <c r="D29" s="5">
         <f t="shared" si="1"/>
-        <v>-5</v>
-      </c>
-      <c r="D29" s="5">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*B29/$C$16/$C$10)</f>
         <v>369.00364041261741</v>
       </c>
       <c r="E29" s="7">
+        <f t="shared" si="7"/>
+        <v>2.75</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="2"/>
+        <v>355.78331889503676</v>
+      </c>
+      <c r="G29" s="7">
+        <f t="shared" si="8"/>
+        <v>1.375</v>
+      </c>
+      <c r="H29" s="3">
         <f t="shared" si="3"/>
-        <v>2.75</v>
-      </c>
-      <c r="F29" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E29/$C$16/$C$10)</f>
-        <v>355.78331889503676</v>
-      </c>
-      <c r="G29" s="7">
+        <v>331.47664987673392</v>
+      </c>
+      <c r="I29" s="7">
+        <f t="shared" si="10"/>
+        <v>0.6875</v>
+      </c>
+      <c r="J29" s="55">
+        <f t="shared" si="9"/>
+        <v>4.3125</v>
+      </c>
+      <c r="K29" s="3">
         <f t="shared" si="4"/>
-        <v>1.375</v>
-      </c>
-      <c r="H29" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G29/$C$16/$C$10)</f>
-        <v>331.47664987673392</v>
-      </c>
-      <c r="I29" s="7">
-        <f t="shared" si="6"/>
-        <v>0.6875</v>
-      </c>
-      <c r="J29" s="55">
-        <f t="shared" si="5"/>
-        <v>4.3125</v>
-      </c>
-      <c r="K29" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I29/$C$16/$C$10)</f>
         <v>308.59510078757296</v>
       </c>
       <c r="V29">
@@ -15880,31 +15880,31 @@
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
       <c r="E30" s="7">
+        <f t="shared" si="7"/>
+        <v>3.25</v>
+      </c>
+      <c r="F30" s="21">
+        <f t="shared" si="2"/>
+        <v>360.51766815224761</v>
+      </c>
+      <c r="G30" s="7">
+        <f t="shared" si="8"/>
+        <v>1.625</v>
+      </c>
+      <c r="H30" s="3">
         <f t="shared" si="3"/>
-        <v>3.25</v>
-      </c>
-      <c r="F30" s="21">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E30/$C$16/$C$10)</f>
-        <v>360.51766815224761</v>
-      </c>
-      <c r="G30" s="7">
+        <v>337.60800814845572</v>
+      </c>
+      <c r="I30" s="7">
+        <f t="shared" si="10"/>
+        <v>0.8125</v>
+      </c>
+      <c r="J30" s="55">
+        <f t="shared" si="9"/>
+        <v>4.1875</v>
+      </c>
+      <c r="K30" s="3">
         <f t="shared" si="4"/>
-        <v>1.625</v>
-      </c>
-      <c r="H30" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G30/$C$16/$C$10)</f>
-        <v>337.60800814845572</v>
-      </c>
-      <c r="I30" s="7">
-        <f t="shared" si="6"/>
-        <v>0.8125</v>
-      </c>
-      <c r="J30" s="55">
-        <f t="shared" si="5"/>
-        <v>4.1875</v>
-      </c>
-      <c r="K30" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I30/$C$16/$C$10)</f>
         <v>313.53289519647547</v>
       </c>
       <c r="V30">
@@ -15934,31 +15934,31 @@
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
       <c r="E31" s="7">
+        <f t="shared" si="7"/>
+        <v>3.75</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="2"/>
+        <v>363.96138146389211</v>
+      </c>
+      <c r="G31" s="7">
+        <f t="shared" si="8"/>
+        <v>1.875</v>
+      </c>
+      <c r="H31" s="3">
         <f t="shared" si="3"/>
-        <v>3.75</v>
-      </c>
-      <c r="F31" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E31/$C$16/$C$10)</f>
-        <v>363.96138146389211</v>
-      </c>
-      <c r="G31" s="7">
+        <v>342.83726581763381</v>
+      </c>
+      <c r="I31" s="7">
+        <f t="shared" si="10"/>
+        <v>0.9375</v>
+      </c>
+      <c r="J31" s="55">
+        <f t="shared" si="9"/>
+        <v>4.0625</v>
+      </c>
+      <c r="K31" s="3">
         <f t="shared" si="4"/>
-        <v>1.875</v>
-      </c>
-      <c r="H31" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G31/$C$16/$C$10)</f>
-        <v>342.83726581763381</v>
-      </c>
-      <c r="I31" s="7">
-        <f t="shared" si="6"/>
-        <v>0.9375</v>
-      </c>
-      <c r="J31" s="55">
-        <f t="shared" si="5"/>
-        <v>4.0625</v>
-      </c>
-      <c r="K31" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I31/$C$16/$C$10)</f>
         <v>318.09299846307812</v>
       </c>
       <c r="V31">
@@ -15988,31 +15988,31 @@
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
       <c r="E32" s="7">
+        <f t="shared" si="7"/>
+        <v>4.25</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="2"/>
+        <v>366.46630045666285</v>
+      </c>
+      <c r="G32" s="7">
+        <f t="shared" si="8"/>
+        <v>2.125</v>
+      </c>
+      <c r="H32" s="3">
         <f t="shared" si="3"/>
-        <v>4.25</v>
-      </c>
-      <c r="F32" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E32/$C$16/$C$10)</f>
-        <v>366.46630045666285</v>
-      </c>
-      <c r="G32" s="7">
+        <v>347.29714804255218</v>
+      </c>
+      <c r="I32" s="7">
+        <f t="shared" si="10"/>
+        <v>1.0625</v>
+      </c>
+      <c r="J32" s="55">
+        <f t="shared" si="9"/>
+        <v>3.9375</v>
+      </c>
+      <c r="K32" s="3">
         <f t="shared" si="4"/>
-        <v>2.125</v>
-      </c>
-      <c r="H32" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G32/$C$16/$C$10)</f>
-        <v>347.29714804255218</v>
-      </c>
-      <c r="I32" s="7">
-        <f t="shared" si="6"/>
-        <v>1.0625</v>
-      </c>
-      <c r="J32" s="55">
-        <f t="shared" si="5"/>
-        <v>3.9375</v>
-      </c>
-      <c r="K32" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I32/$C$16/$C$10)</f>
         <v>322.30430012533236</v>
       </c>
       <c r="V32">
@@ -16042,31 +16042,31 @@
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
       <c r="E33" s="7">
+        <f t="shared" si="7"/>
+        <v>4.75</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="2"/>
+        <v>368.28835084022035</v>
+      </c>
+      <c r="G33" s="7">
+        <f t="shared" si="8"/>
+        <v>2.375</v>
+      </c>
+      <c r="H33" s="3">
         <f t="shared" si="3"/>
-        <v>4.75</v>
-      </c>
-      <c r="F33" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E33/$C$16/$C$10)</f>
-        <v>368.28835084022035</v>
-      </c>
-      <c r="G33" s="7">
+        <v>351.10085226186811</v>
+      </c>
+      <c r="I33" s="7">
+        <f t="shared" si="10"/>
+        <v>1.1875</v>
+      </c>
+      <c r="J33" s="55">
+        <f t="shared" si="9"/>
+        <v>3.8125</v>
+      </c>
+      <c r="K33" s="3">
         <f t="shared" si="4"/>
-        <v>2.375</v>
-      </c>
-      <c r="H33" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G33/$C$16/$C$10)</f>
-        <v>351.10085226186811</v>
-      </c>
-      <c r="I33" s="7">
-        <f t="shared" si="6"/>
-        <v>1.1875</v>
-      </c>
-      <c r="J33" s="55">
-        <f t="shared" si="5"/>
-        <v>3.8125</v>
-      </c>
-      <c r="K33" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I33/$C$16/$C$10)</f>
         <v>326.19347996483145</v>
       </c>
       <c r="V33">
@@ -16100,27 +16100,27 @@
         <v>5</v>
       </c>
       <c r="F34" s="5">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*E34/$C$16/$C$10)</f>
+        <f t="shared" si="2"/>
         <v>369.00364041261741</v>
       </c>
       <c r="G34" s="7">
+        <f t="shared" si="8"/>
+        <v>2.625</v>
+      </c>
+      <c r="H34" s="3">
+        <f t="shared" si="3"/>
+        <v>354.34492128844568</v>
+      </c>
+      <c r="I34" s="7">
+        <f t="shared" si="10"/>
+        <v>1.3125</v>
+      </c>
+      <c r="J34" s="55">
+        <f t="shared" si="9"/>
+        <v>3.6875</v>
+      </c>
+      <c r="K34" s="3">
         <f t="shared" si="4"/>
-        <v>2.625</v>
-      </c>
-      <c r="H34" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G34/$C$16/$C$10)</f>
-        <v>354.34492128844568</v>
-      </c>
-      <c r="I34" s="7">
-        <f t="shared" si="6"/>
-        <v>1.3125</v>
-      </c>
-      <c r="J34" s="55">
-        <f t="shared" si="5"/>
-        <v>3.6875</v>
-      </c>
-      <c r="K34" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I34/$C$16/$C$10)</f>
         <v>329.78517703073805</v>
       </c>
       <c r="V34">
@@ -16152,23 +16152,23 @@
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
       <c r="G35" s="7">
+        <f t="shared" si="8"/>
+        <v>2.875</v>
+      </c>
+      <c r="H35" s="3">
+        <f t="shared" si="3"/>
+        <v>357.11169368777087</v>
+      </c>
+      <c r="I35" s="7">
+        <f t="shared" si="10"/>
+        <v>1.4375</v>
+      </c>
+      <c r="J35" s="55">
+        <f t="shared" si="9"/>
+        <v>3.5625</v>
+      </c>
+      <c r="K35" s="3">
         <f t="shared" si="4"/>
-        <v>2.875</v>
-      </c>
-      <c r="H35" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G35/$C$16/$C$10)</f>
-        <v>357.11169368777087</v>
-      </c>
-      <c r="I35" s="7">
-        <f t="shared" si="6"/>
-        <v>1.4375</v>
-      </c>
-      <c r="J35" s="55">
-        <f t="shared" si="5"/>
-        <v>3.5625</v>
-      </c>
-      <c r="K35" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I35/$C$16/$C$10)</f>
         <v>333.102145735097</v>
       </c>
       <c r="V35">
@@ -16200,23 +16200,23 @@
       <c r="E36" s="15"/>
       <c r="F36" s="15"/>
       <c r="G36" s="7">
+        <f t="shared" si="8"/>
+        <v>3.125</v>
+      </c>
+      <c r="H36" s="3">
+        <f t="shared" si="3"/>
+        <v>359.47139363464396</v>
+      </c>
+      <c r="I36" s="7">
+        <f t="shared" si="10"/>
+        <v>1.5625</v>
+      </c>
+      <c r="J36" s="55">
+        <f t="shared" si="9"/>
+        <v>3.4375</v>
+      </c>
+      <c r="K36" s="3">
         <f t="shared" si="4"/>
-        <v>3.125</v>
-      </c>
-      <c r="H36" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G36/$C$16/$C$10)</f>
-        <v>359.47139363464396</v>
-      </c>
-      <c r="I36" s="7">
-        <f t="shared" si="6"/>
-        <v>1.5625</v>
-      </c>
-      <c r="J36" s="55">
-        <f t="shared" si="5"/>
-        <v>3.4375</v>
-      </c>
-      <c r="K36" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I36/$C$16/$C$10)</f>
         <v>336.16540000844128</v>
       </c>
       <c r="V36">
@@ -16248,23 +16248,23 @@
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
       <c r="G37" s="7">
+        <f t="shared" si="8"/>
+        <v>3.375</v>
+      </c>
+      <c r="H37" s="3">
+        <f t="shared" si="3"/>
+        <v>361.48391329134967</v>
+      </c>
+      <c r="I37" s="7">
+        <f t="shared" si="10"/>
+        <v>1.6875</v>
+      </c>
+      <c r="J37" s="55">
+        <f t="shared" si="9"/>
+        <v>3.3125</v>
+      </c>
+      <c r="K37" s="3">
         <f t="shared" si="4"/>
-        <v>3.375</v>
-      </c>
-      <c r="H37" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G37/$C$16/$C$10)</f>
-        <v>361.48391329134967</v>
-      </c>
-      <c r="I37" s="7">
-        <f t="shared" si="6"/>
-        <v>1.6875</v>
-      </c>
-      <c r="J37" s="55">
-        <f t="shared" si="5"/>
-        <v>3.3125</v>
-      </c>
-      <c r="K37" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I37/$C$16/$C$10)</f>
         <v>338.99434642895801</v>
       </c>
       <c r="V37">
@@ -16296,23 +16296,23 @@
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
       <c r="G38" s="7">
+        <f t="shared" si="8"/>
+        <v>3.625</v>
+      </c>
+      <c r="H38" s="3">
+        <f t="shared" si="3"/>
+        <v>363.20033294631213</v>
+      </c>
+      <c r="I38" s="7">
+        <f t="shared" si="10"/>
+        <v>1.8125</v>
+      </c>
+      <c r="J38" s="55">
+        <f t="shared" si="9"/>
+        <v>3.1875</v>
+      </c>
+      <c r="K38" s="3">
         <f t="shared" si="4"/>
-        <v>3.625</v>
-      </c>
-      <c r="H38" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G38/$C$16/$C$10)</f>
-        <v>363.20033294631213</v>
-      </c>
-      <c r="I38" s="7">
-        <f t="shared" si="6"/>
-        <v>1.8125</v>
-      </c>
-      <c r="J38" s="55">
-        <f t="shared" si="5"/>
-        <v>3.1875</v>
-      </c>
-      <c r="K38" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I38/$C$16/$C$10)</f>
         <v>341.60690716862428</v>
       </c>
       <c r="V38">
@@ -16344,23 +16344,23 @@
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
       <c r="G39" s="7">
+        <f t="shared" si="8"/>
+        <v>3.875</v>
+      </c>
+      <c r="H39" s="3">
+        <f t="shared" si="3"/>
+        <v>364.66421749627176</v>
+      </c>
+      <c r="I39" s="7">
+        <f t="shared" si="10"/>
+        <v>1.9375</v>
+      </c>
+      <c r="J39" s="55">
+        <f t="shared" si="9"/>
+        <v>3.0625</v>
+      </c>
+      <c r="K39" s="3">
         <f t="shared" si="4"/>
-        <v>3.875</v>
-      </c>
-      <c r="H39" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G39/$C$16/$C$10)</f>
-        <v>364.66421749627176</v>
-      </c>
-      <c r="I39" s="7">
-        <f t="shared" si="6"/>
-        <v>1.9375</v>
-      </c>
-      <c r="J39" s="55">
-        <f t="shared" si="5"/>
-        <v>3.0625</v>
-      </c>
-      <c r="K39" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I39/$C$16/$C$10)</f>
         <v>344.01963353521239</v>
       </c>
       <c r="V39">
@@ -16392,23 +16392,23 @@
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
       <c r="G40" s="7">
+        <f t="shared" si="8"/>
+        <v>4.125</v>
+      </c>
+      <c r="H40" s="3">
+        <f t="shared" si="3"/>
+        <v>365.91272217833756</v>
+      </c>
+      <c r="I40" s="7">
+        <f t="shared" si="10"/>
+        <v>2.0625</v>
+      </c>
+      <c r="J40" s="55">
+        <f t="shared" si="9"/>
+        <v>2.9375</v>
+      </c>
+      <c r="K40" s="3">
         <f t="shared" si="4"/>
-        <v>4.125</v>
-      </c>
-      <c r="H40" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G40/$C$16/$C$10)</f>
-        <v>365.91272217833756</v>
-      </c>
-      <c r="I40" s="7">
-        <f t="shared" si="6"/>
-        <v>2.0625</v>
-      </c>
-      <c r="J40" s="55">
-        <f t="shared" si="5"/>
-        <v>2.9375</v>
-      </c>
-      <c r="K40" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I40/$C$16/$C$10)</f>
         <v>346.24781082948374</v>
       </c>
       <c r="V40">
@@ -16440,23 +16440,23 @@
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
       <c r="G41" s="7">
+        <f t="shared" si="8"/>
+        <v>4.375</v>
+      </c>
+      <c r="H41" s="3">
+        <f t="shared" si="3"/>
+        <v>366.97753561679031</v>
+      </c>
+      <c r="I41" s="7">
+        <f t="shared" si="10"/>
+        <v>2.1875</v>
+      </c>
+      <c r="J41" s="55">
+        <f t="shared" si="9"/>
+        <v>2.8125</v>
+      </c>
+      <c r="K41" s="3">
         <f t="shared" si="4"/>
-        <v>4.375</v>
-      </c>
-      <c r="H41" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G41/$C$16/$C$10)</f>
-        <v>366.97753561679031</v>
-      </c>
-      <c r="I41" s="7">
-        <f t="shared" si="6"/>
-        <v>2.1875</v>
-      </c>
-      <c r="J41" s="55">
-        <f t="shared" si="5"/>
-        <v>2.8125</v>
-      </c>
-      <c r="K41" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I41/$C$16/$C$10)</f>
         <v>348.30555518187271</v>
       </c>
       <c r="V41">
@@ -16488,23 +16488,23 @@
       <c r="E42" s="15"/>
       <c r="F42" s="15"/>
       <c r="G42" s="7">
+        <f t="shared" si="8"/>
+        <v>4.625</v>
+      </c>
+      <c r="H42" s="3">
+        <f t="shared" si="3"/>
+        <v>367.88568412035329</v>
+      </c>
+      <c r="I42" s="7">
+        <f t="shared" si="10"/>
+        <v>2.3125</v>
+      </c>
+      <c r="J42" s="55">
+        <f t="shared" si="9"/>
+        <v>2.6875</v>
+      </c>
+      <c r="K42" s="3">
         <f t="shared" si="4"/>
-        <v>4.625</v>
-      </c>
-      <c r="H42" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G42/$C$16/$C$10)</f>
-        <v>367.88568412035329</v>
-      </c>
-      <c r="I42" s="7">
-        <f t="shared" si="6"/>
-        <v>2.3125</v>
-      </c>
-      <c r="J42" s="55">
-        <f t="shared" si="5"/>
-        <v>2.6875</v>
-      </c>
-      <c r="K42" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I42/$C$16/$C$10)</f>
         <v>350.20590298214654</v>
       </c>
       <c r="V42">
@@ -16536,23 +16536,23 @@
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
       <c r="G43" s="7">
+        <f t="shared" si="8"/>
+        <v>4.875</v>
+      </c>
+      <c r="H43" s="34">
+        <f t="shared" si="3"/>
+        <v>368.66021764401177</v>
+      </c>
+      <c r="I43" s="7">
+        <f t="shared" si="10"/>
+        <v>2.4375</v>
+      </c>
+      <c r="J43" s="55">
+        <f t="shared" si="9"/>
+        <v>2.5625</v>
+      </c>
+      <c r="K43" s="34">
         <f t="shared" si="4"/>
-        <v>4.875</v>
-      </c>
-      <c r="H43" s="34">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G43/$C$16/$C$10)</f>
-        <v>368.66021764401177</v>
-      </c>
-      <c r="I43" s="7">
-        <f t="shared" si="6"/>
-        <v>2.4375</v>
-      </c>
-      <c r="J43" s="55">
-        <f t="shared" si="5"/>
-        <v>2.5625</v>
-      </c>
-      <c r="K43" s="34">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I43/$C$16/$C$10)</f>
         <v>351.9608934686047</v>
       </c>
       <c r="V43">
@@ -16588,19 +16588,19 @@
         <v>5</v>
       </c>
       <c r="H44" s="37">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*G44/$C$16/$C$10)</f>
+        <f t="shared" si="3"/>
         <v>369.00364041261741</v>
       </c>
       <c r="I44" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.5625</v>
       </c>
       <c r="J44" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2.4375</v>
       </c>
       <c r="K44" s="35">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I44/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>353.58164500004261</v>
       </c>
       <c r="V44">
@@ -16638,11 +16638,11 @@
         <v>2.6875</v>
       </c>
       <c r="J45" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2.3125</v>
       </c>
       <c r="K45" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I45/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>355.07842549368496</v>
       </c>
       <c r="V45">
@@ -16680,11 +16680,11 @@
         <v>2.8125</v>
       </c>
       <c r="J46" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2.1875</v>
       </c>
       <c r="K46" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I46/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>356.46071747533159</v>
       </c>
       <c r="V46">
@@ -16718,15 +16718,15 @@
       <c r="G47" s="15"/>
       <c r="H47" s="15"/>
       <c r="I47" s="7">
-        <f t="shared" ref="I47:I63" si="8">I46+$I$8</f>
+        <f t="shared" ref="I47:I63" si="12">I46+$I$8</f>
         <v>2.9375</v>
       </c>
       <c r="J47" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2.0625</v>
       </c>
       <c r="K47" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I47/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>357.7372781538283</v>
       </c>
       <c r="V47">
@@ -16760,15 +16760,15 @@
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
       <c r="I48" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.0625</v>
       </c>
       <c r="J48" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.9375</v>
       </c>
       <c r="K48" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I48/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>358.91619490044985</v>
       </c>
       <c r="V48">
@@ -16802,15 +16802,15 @@
       <c r="G49" s="15"/>
       <c r="H49" s="15"/>
       <c r="I49" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.1875</v>
       </c>
       <c r="J49" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.8125</v>
       </c>
       <c r="K49" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I49/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>360.00493648467392</v>
       </c>
       <c r="V49">
@@ -16844,15 +16844,15 @@
       <c r="G50" s="15"/>
       <c r="H50" s="15"/>
       <c r="I50" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.3125</v>
       </c>
       <c r="J50" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.6875</v>
       </c>
       <c r="K50" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I50/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>361.01040039093857</v>
       </c>
       <c r="V50">
@@ -16886,15 +16886,15 @@
       <c r="G51" s="15"/>
       <c r="H51" s="15"/>
       <c r="I51" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.4375</v>
       </c>
       <c r="J51" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.5625</v>
       </c>
       <c r="K51" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I51/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>361.93895651614741</v>
       </c>
       <c r="V51">
@@ -16928,15 +16928,15 @@
       <c r="G52" s="15"/>
       <c r="H52" s="15"/>
       <c r="I52" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.5625</v>
       </c>
       <c r="J52" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.4375</v>
       </c>
       <c r="K52" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I52/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>362.79648752476015</v>
       </c>
       <c r="V52">
@@ -16970,15 +16970,15 @@
       <c r="G53" s="15"/>
       <c r="H53" s="15"/>
       <c r="I53" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.6875</v>
       </c>
       <c r="J53" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.3125</v>
       </c>
       <c r="K53" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I53/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>363.58842611712805</v>
       </c>
       <c r="V53">
@@ -17012,15 +17012,15 @@
       <c r="G54" s="15"/>
       <c r="H54" s="15"/>
       <c r="I54" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.8125</v>
       </c>
       <c r="J54" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.1875</v>
       </c>
       <c r="K54" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I54/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>364.3197894471798</v>
       </c>
       <c r="V54">
@@ -17054,15 +17054,15 @@
       <c r="G55" s="15"/>
       <c r="H55" s="15"/>
       <c r="I55" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3.9375</v>
       </c>
       <c r="J55" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1.0625</v>
       </c>
       <c r="K55" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I55/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>364.99521090750409</v>
       </c>
       <c r="V55">
@@ -17096,15 +17096,15 @@
       <c r="G56" s="15"/>
       <c r="H56" s="15"/>
       <c r="I56" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.0625</v>
       </c>
       <c r="J56" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.9375</v>
       </c>
       <c r="K56" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I56/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>365.61896948319645</v>
       </c>
       <c r="V56">
@@ -17138,15 +17138,15 @@
       <c r="G57" s="15"/>
       <c r="H57" s="15"/>
       <c r="I57" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.1875</v>
       </c>
       <c r="J57" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.8125</v>
       </c>
       <c r="K57" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I57/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>366.1950168604339</v>
       </c>
       <c r="V57">
@@ -17180,15 +17180,15 @@
       <c r="G58" s="15"/>
       <c r="H58" s="15"/>
       <c r="I58" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.3125</v>
       </c>
       <c r="J58" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.6875</v>
       </c>
       <c r="K58" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I58/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>366.72700246151976</v>
       </c>
       <c r="V58">
@@ -17222,15 +17222,15 @@
       <c r="G59" s="15"/>
       <c r="H59" s="15"/>
       <c r="I59" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.4375</v>
       </c>
       <c r="J59" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.5625</v>
       </c>
       <c r="K59" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I59/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>367.21829656500114</v>
       </c>
       <c r="V59">
@@ -17264,15 +17264,15 @@
       <c r="G60" s="15"/>
       <c r="H60" s="15"/>
       <c r="I60" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.5625</v>
       </c>
       <c r="J60" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.4375</v>
       </c>
       <c r="K60" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I60/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>367.67201165733246</v>
       </c>
       <c r="V60">
@@ -17306,15 +17306,15 @@
       <c r="G61" s="15"/>
       <c r="H61" s="15"/>
       <c r="I61" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.6875</v>
       </c>
       <c r="J61" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.3125</v>
       </c>
       <c r="K61" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I61/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>368.09102215135317</v>
       </c>
       <c r="V61">
@@ -17348,15 +17348,15 @@
       <c r="G62" s="15"/>
       <c r="H62" s="15"/>
       <c r="I62" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.8125</v>
       </c>
       <c r="J62" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0.1875</v>
       </c>
       <c r="K62" s="3">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I62/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>368.4779825965025</v>
       </c>
       <c r="V62">
@@ -17390,15 +17390,15 @@
       <c r="G63" s="15"/>
       <c r="H63" s="15"/>
       <c r="I63" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.9375</v>
       </c>
       <c r="J63" s="55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>6.25E-2</v>
       </c>
       <c r="K63" s="34">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I63/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>368.83534449613728</v>
       </c>
       <c r="L63">
@@ -17444,7 +17444,7 @@
         <v>0</v>
       </c>
       <c r="K64" s="37">
-        <f>$C$14-($C$14-$C$11)*EXP(-$C$13*$C$15*I64/$C$16/$C$10)</f>
+        <f t="shared" si="4"/>
         <v>369.00364041261741</v>
       </c>
       <c r="L64">

</xml_diff>